<commit_message>
Added ALU Control unit, and modified ALU
</commit_message>
<xml_diff>
--- a/IS.xlsx
+++ b/IS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Okasha\Documents\modifiedMIPS\modifiedMIPS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56AC4CD8-CF20-411B-9550-88339E28D912}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FDE05AD-D82D-44F1-88BC-EDEAE0D20EFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-5940" yWindow="3405" windowWidth="11970" windowHeight="10200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instr. Formats" sheetId="2" r:id="rId1"/>
@@ -1056,7 +1056,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1105,6 +1105,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1544,7 +1545,7 @@
   <dimension ref="B2:N20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P23" sqref="P23"/>
+      <selection activeCell="C8" sqref="C8:N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1877,8 +1878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:X37"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21:H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2432,36 +2433,37 @@
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
     </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B17">
+    <row r="17" spans="2:18" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="12">
         <f>B16+1</f>
         <v>14</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="22" t="s">
         <v>245</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F17" s="22" t="s">
         <v>247</v>
       </c>
-      <c r="H17" s="9" t="s">
+      <c r="G17" s="22"/>
+      <c r="H17" s="22" t="s">
         <v>255</v>
       </c>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
-      <c r="O17" s="1"/>
-      <c r="P17" s="1"/>
-      <c r="Q17" s="1"/>
-      <c r="R17" s="1"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="22"/>
+      <c r="M17" s="22"/>
+      <c r="N17" s="22"/>
+      <c r="O17" s="22"/>
+      <c r="P17" s="22"/>
+      <c r="Q17" s="22"/>
+      <c r="R17" s="22"/>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B18">
@@ -3118,8 +3120,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A3:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Major changes to structure of pipeline, Register File added 3rd output, modified some other units
</commit_message>
<xml_diff>
--- a/IS.xlsx
+++ b/IS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Okasha\Documents\modifiedMIPS\modifiedMIPS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FDE05AD-D82D-44F1-88BC-EDEAE0D20EFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6F6A9C1-EDD9-46FE-8377-96823AFDD8E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5940" yWindow="3405" windowWidth="11970" windowHeight="10200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3405" windowWidth="11970" windowHeight="10200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instr. Formats" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="304">
   <si>
     <t>FORMAT</t>
   </si>
@@ -922,6 +922,36 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>OPCODE zay el kheleg</t>
+  </si>
+  <si>
+    <t>000011</t>
+  </si>
+  <si>
+    <t>001001</t>
+  </si>
+  <si>
+    <t>001000</t>
+  </si>
+  <si>
+    <t>001100</t>
+  </si>
+  <si>
+    <t>000101</t>
+  </si>
+  <si>
+    <t>000100</t>
+  </si>
+  <si>
+    <t>ALU OPc</t>
+  </si>
+  <si>
+    <t>010</t>
+  </si>
+  <si>
+    <t>000</t>
   </si>
 </sst>
 </file>
@@ -960,7 +990,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -988,6 +1018,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1056,7 +1092,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1105,12 +1141,25 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="30">
+  <dxfs count="32">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
@@ -1225,55 +1274,57 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="B3:R29" totalsRowShown="0" headerRowDxfId="29">
-  <tableColumns count="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="B3:T29" totalsRowShown="0" headerRowDxfId="31">
+  <tableColumns count="19">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="No.">
       <calculatedColumnFormula>B3+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="NAME" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="MNEMONIC" dataDxfId="27"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="FORMAT" dataDxfId="26"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="OPERATION (in Verilog)" dataDxfId="25"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Note" dataDxfId="24"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="OPCODE/ FUNCT(Hex)" dataDxfId="23"/>
-    <tableColumn id="8" xr3:uid="{EE7F7B4D-DDD2-489C-8627-F67632B6806B}" name="ALU OP" dataDxfId="22"/>
-    <tableColumn id="9" xr3:uid="{AAFC0202-CB70-4B1A-9AF4-7E75B12C923B}" name="MemWrite" dataDxfId="21"/>
-    <tableColumn id="10" xr3:uid="{D4CA723B-8BCB-47DF-81D6-CE8E45FA7F18}" name="RegWrite" dataDxfId="20"/>
-    <tableColumn id="11" xr3:uid="{F06965CD-61B4-44BE-AFFB-16FD9D4BB004}" name="ALUs" dataDxfId="19"/>
-    <tableColumn id="12" xr3:uid="{BAC6153E-232C-4723-973E-5135B68C73F1}" name="Float" dataDxfId="18"/>
-    <tableColumn id="13" xr3:uid="{9E280564-ACAE-4469-8DE1-F31D0FCA6F71}" name="RegDst" dataDxfId="17"/>
-    <tableColumn id="14" xr3:uid="{856F9B53-AECE-404A-BB0B-7759D6599868}" name="HiLoWrite" dataDxfId="16"/>
-    <tableColumn id="15" xr3:uid="{C2001F97-A3F7-4884-9E5D-BC4ACC8AE232}" name="HL" dataDxfId="15"/>
-    <tableColumn id="16" xr3:uid="{8BA1CFC8-404A-4666-B7C9-97101DA879B4}" name="WBSrc" dataDxfId="14"/>
-    <tableColumn id="17" xr3:uid="{69D73963-7CBA-4A8D-8D02-94AC9142117F}" name="ALUc" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="NAME" dataDxfId="30"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="MNEMONIC" dataDxfId="29"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="FORMAT" dataDxfId="28"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="OPERATION (in Verilog)" dataDxfId="27"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Note" dataDxfId="26"/>
+    <tableColumn id="18" xr3:uid="{DFACAFC1-11FF-491F-9AB8-4002EB4348F8}" name="OPCODE zay el kheleg" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="OPCODE/ FUNCT(Hex)" dataDxfId="25"/>
+    <tableColumn id="19" xr3:uid="{7A4C5E34-6C04-4A0B-87EB-FBF54DC3C353}" name="ALU OPc" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{EE7F7B4D-DDD2-489C-8627-F67632B6806B}" name="ALU OP" dataDxfId="24"/>
+    <tableColumn id="9" xr3:uid="{AAFC0202-CB70-4B1A-9AF4-7E75B12C923B}" name="MemWrite" dataDxfId="23"/>
+    <tableColumn id="10" xr3:uid="{D4CA723B-8BCB-47DF-81D6-CE8E45FA7F18}" name="RegWrite" dataDxfId="22"/>
+    <tableColumn id="11" xr3:uid="{F06965CD-61B4-44BE-AFFB-16FD9D4BB004}" name="ALUs" dataDxfId="21"/>
+    <tableColumn id="12" xr3:uid="{BAC6153E-232C-4723-973E-5135B68C73F1}" name="Float" dataDxfId="20"/>
+    <tableColumn id="13" xr3:uid="{9E280564-ACAE-4469-8DE1-F31D0FCA6F71}" name="RegDst" dataDxfId="19"/>
+    <tableColumn id="14" xr3:uid="{856F9B53-AECE-404A-BB0B-7759D6599868}" name="HiLoWrite" dataDxfId="18"/>
+    <tableColumn id="15" xr3:uid="{C2001F97-A3F7-4884-9E5D-BC4ACC8AE232}" name="HL" dataDxfId="17"/>
+    <tableColumn id="16" xr3:uid="{8BA1CFC8-404A-4666-B7C9-97101DA879B4}" name="WBSrc" dataDxfId="16"/>
+    <tableColumn id="17" xr3:uid="{69D73963-7CBA-4A8D-8D02-94AC9142117F}" name="ALUc" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="B3:E14" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="B3:E14" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="B3:E14" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="NAME" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="NUMBER" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="USE" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="PRESERVED ACROSS A CALL?" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="NAME" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="NUMBER" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="USE" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="PRESERVED ACROSS A CALL?" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table3" displayName="Table3" ref="B3:G27" totalsRowShown="0" headerRowDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table3" displayName="Table3" ref="B3:G27" totalsRowShown="0" headerRowDxfId="8">
   <autoFilter ref="B3:G27" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="NAME" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="MNEMONIC" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="FORMAT" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="OPERATION" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Note" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Opcode/ FMT /FT/ FUNCT(Hex)" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="NAME" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="MNEMONIC" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="FORMAT" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="OPERATION" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Note" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Opcode/ FMT /FT/ FUNCT(Hex)" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1545,7 +1596,7 @@
   <dimension ref="B2:N20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8:N9"/>
+      <selection activeCell="K5" sqref="K5:L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1847,18 +1898,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:N11"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="I8:N8"/>
     <mergeCell ref="M16:N16"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="E19:F19"/>
@@ -1869,6 +1908,18 @@
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="I16:J16"/>
     <mergeCell ref="K16:L16"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:N11"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="I8:N8"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1876,10 +1927,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B2:X37"/>
+  <dimension ref="B2:Z37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21:H24"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1889,16 +1940,16 @@
     <col min="5" max="5" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29" style="9" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="29" style="9" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" style="9" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="J2" s="20" t="s">
+    <row r="2" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="L2" s="20" t="s">
         <v>281</v>
       </c>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
       <c r="M2" s="20"/>
       <c r="N2" s="20"/>
       <c r="O2" s="20"/>
@@ -1911,8 +1962,10 @@
       <c r="V2" s="20"/>
       <c r="W2" s="20"/>
       <c r="X2" s="20"/>
-    </row>
-    <row r="3" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Y2" s="20"/>
+      <c r="Z2" s="20"/>
+    </row>
+    <row r="3" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>5</v>
       </c>
@@ -1931,92 +1984,104 @@
       <c r="G3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="I3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="J3" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="K3" s="14" t="s">
         <v>276</v>
       </c>
-      <c r="J3" s="15" t="s">
+      <c r="L3" s="15" t="s">
         <v>282</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="S3" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="T3" s="1" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="4" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B4">
+    <row r="4" spans="2:26" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="22">
         <v>1</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="23" t="s">
+        <v>295</v>
+      </c>
+      <c r="I4" s="23" t="s">
         <v>252</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="23" t="s">
+        <v>302</v>
+      </c>
+      <c r="K4" s="23" t="s">
         <v>277</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="L4" s="23" t="s">
         <v>291</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="M4" s="23" t="s">
         <v>292</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="N4" s="23" t="s">
         <v>291</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="O4" s="23" t="s">
         <v>291</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="P4" s="23" t="s">
         <v>291</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="Q4" s="23" t="s">
         <v>291</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="R4" s="23" t="s">
         <v>293</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="S4" s="23" t="s">
         <v>291</v>
       </c>
-      <c r="R4" s="1"/>
-    </row>
-    <row r="5" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="T4" s="23"/>
+    </row>
+    <row r="5" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B5">
         <f>B4+1</f>
         <v>2</v>
@@ -2036,14 +2101,15 @@
       <c r="G5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="I5" s="9" t="s">
         <v>240</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
@@ -2051,8 +2117,10 @@
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
-    </row>
-    <row r="6" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+    </row>
+    <row r="6" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B6">
         <f t="shared" ref="B6:B29" si="0">B5+1</f>
         <v>3</v>
@@ -2072,14 +2140,15 @@
       <c r="G6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="I6" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
@@ -2087,41 +2156,50 @@
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
-    </row>
-    <row r="7" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B7">
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+    </row>
+    <row r="7" spans="2:26" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="22">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="G7" s="23"/>
+      <c r="H7" s="23" t="s">
+        <v>295</v>
+      </c>
+      <c r="I7" s="23" t="s">
         <v>253</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="J7" s="23" t="s">
+        <v>302</v>
+      </c>
+      <c r="K7" s="23" t="s">
         <v>278</v>
       </c>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="1"/>
-      <c r="R7" s="1"/>
-    </row>
-    <row r="8" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="L7" s="23"/>
+      <c r="M7" s="23"/>
+      <c r="N7" s="23"/>
+      <c r="O7" s="23"/>
+      <c r="P7" s="23"/>
+      <c r="Q7" s="23"/>
+      <c r="R7" s="23"/>
+      <c r="S7" s="23"/>
+      <c r="T7" s="23"/>
+    </row>
+    <row r="8" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B8">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -2141,14 +2219,15 @@
       <c r="G8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="H8" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="I8" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="K8" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
@@ -2156,8 +2235,10 @@
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
-    </row>
-    <row r="9" spans="2:24" ht="30" x14ac:dyDescent="0.25">
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+    </row>
+    <row r="9" spans="2:26" ht="30" x14ac:dyDescent="0.25">
       <c r="B9">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -2177,14 +2258,15 @@
       <c r="G9" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="H9" s="9" t="s">
+      <c r="H9" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="I9" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="K9" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
@@ -2192,8 +2274,10 @@
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
-    </row>
-    <row r="10" spans="2:24" ht="30" x14ac:dyDescent="0.25">
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+    </row>
+    <row r="10" spans="2:26" ht="30" x14ac:dyDescent="0.25">
       <c r="B10">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -2213,14 +2297,15 @@
       <c r="G10" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="H10" s="9" t="s">
+      <c r="H10" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="I10" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="K10" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
@@ -2228,8 +2313,10 @@
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
-    </row>
-    <row r="11" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+    </row>
+    <row r="11" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B11">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -2249,11 +2336,9 @@
       <c r="G11" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H11" s="9" t="s">
+      <c r="I11" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
@@ -2262,8 +2347,10 @@
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
-    </row>
-    <row r="12" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+    </row>
+    <row r="12" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B12">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -2283,11 +2370,9 @@
       <c r="G12" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H12" s="9" t="s">
+      <c r="I12" s="9" t="s">
         <v>265</v>
       </c>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
@@ -2296,8 +2381,10 @@
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
-    </row>
-    <row r="13" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+    </row>
+    <row r="13" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B13">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -2314,14 +2401,12 @@
       <c r="F13" s="9" t="s">
         <v>273</v>
       </c>
-      <c r="H13" s="9" t="s">
+      <c r="I13" s="9" t="s">
         <v>254</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="K13" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
@@ -2329,8 +2414,10 @@
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
-    </row>
-    <row r="14" spans="2:24" ht="30" x14ac:dyDescent="0.25">
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+    </row>
+    <row r="14" spans="2:26" ht="30" x14ac:dyDescent="0.25">
       <c r="B14">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -2350,14 +2437,12 @@
       <c r="G14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H14" s="9" t="s">
+      <c r="I14" s="9" t="s">
         <v>237</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="K14" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
@@ -2365,8 +2450,10 @@
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
-    </row>
-    <row r="15" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+    </row>
+    <row r="15" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B15">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -2383,11 +2470,9 @@
       <c r="F15" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="H15" s="9" t="s">
+      <c r="I15" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
@@ -2396,138 +2481,162 @@
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
-    </row>
-    <row r="16" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B16">
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+    </row>
+    <row r="16" spans="2:26" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="10">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F16" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="G16" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="H16" s="9" t="s">
+      <c r="H16" s="9"/>
+      <c r="I16" s="9" t="s">
         <v>238</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="J16" s="9"/>
+      <c r="K16" s="9" t="s">
         <v>277</v>
       </c>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
-      <c r="Q16" s="1"/>
-      <c r="R16" s="1"/>
-    </row>
-    <row r="17" spans="2:18" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="12">
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="9"/>
+      <c r="S16" s="9"/>
+      <c r="T16" s="9"/>
+    </row>
+    <row r="17" spans="2:20" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="22">
         <f>B16+1</f>
         <v>14</v>
       </c>
-      <c r="C17" s="22" t="s">
+      <c r="C17" s="23" t="s">
         <v>245</v>
       </c>
-      <c r="D17" s="22" t="s">
+      <c r="D17" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="E17" s="22" t="s">
+      <c r="E17" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="22" t="s">
+      <c r="F17" s="23" t="s">
         <v>247</v>
       </c>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22" t="s">
+      <c r="G17" s="23"/>
+      <c r="H17" s="23" t="s">
+        <v>295</v>
+      </c>
+      <c r="I17" s="23" t="s">
         <v>255</v>
       </c>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
-      <c r="K17" s="22"/>
-      <c r="L17" s="22"/>
-      <c r="M17" s="22"/>
-      <c r="N17" s="22"/>
-      <c r="O17" s="22"/>
-      <c r="P17" s="22"/>
-      <c r="Q17" s="22"/>
-      <c r="R17" s="22"/>
-    </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B18">
+      <c r="J17" s="23" t="s">
+        <v>302</v>
+      </c>
+      <c r="K17" s="23"/>
+      <c r="L17" s="23"/>
+      <c r="M17" s="23"/>
+      <c r="N17" s="23"/>
+      <c r="O17" s="23"/>
+      <c r="P17" s="23"/>
+      <c r="Q17" s="23"/>
+      <c r="R17" s="23"/>
+      <c r="S17" s="23"/>
+      <c r="T17" s="23"/>
+    </row>
+    <row r="18" spans="2:20" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="22">
         <f>B16+1</f>
         <v>14</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="F18" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="H18" s="9" t="s">
+      <c r="G18" s="23"/>
+      <c r="H18" s="23" t="s">
+        <v>295</v>
+      </c>
+      <c r="I18" s="23" t="s">
         <v>256</v>
       </c>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
-      <c r="O18" s="1"/>
-      <c r="P18" s="1"/>
-      <c r="Q18" s="1"/>
-      <c r="R18" s="1"/>
-    </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B19">
+      <c r="J18" s="23" t="s">
+        <v>302</v>
+      </c>
+      <c r="K18" s="23"/>
+      <c r="L18" s="23"/>
+      <c r="M18" s="23"/>
+      <c r="N18" s="23"/>
+      <c r="O18" s="23"/>
+      <c r="P18" s="23"/>
+      <c r="Q18" s="23"/>
+      <c r="R18" s="23"/>
+      <c r="S18" s="23"/>
+      <c r="T18" s="23"/>
+    </row>
+    <row r="19" spans="2:20" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="22">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F19" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="H19" s="9" t="s">
+      <c r="G19" s="23"/>
+      <c r="H19" s="23" t="s">
+        <v>295</v>
+      </c>
+      <c r="I19" s="23" t="s">
         <v>257</v>
       </c>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
-      <c r="P19" s="1"/>
-      <c r="Q19" s="1"/>
-      <c r="R19" s="1"/>
-    </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="J19" s="23" t="s">
+        <v>302</v>
+      </c>
+      <c r="K19" s="23"/>
+      <c r="L19" s="23"/>
+      <c r="M19" s="23"/>
+      <c r="N19" s="23"/>
+      <c r="O19" s="23"/>
+      <c r="P19" s="23"/>
+      <c r="Q19" s="23"/>
+      <c r="R19" s="23"/>
+      <c r="S19" s="23"/>
+      <c r="T19" s="23"/>
+    </row>
+    <row r="20" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B20">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2547,11 +2656,9 @@
       <c r="G20" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H20" s="9" t="s">
+      <c r="I20" s="9" t="s">
         <v>239</v>
       </c>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
@@ -2560,135 +2667,164 @@
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
-    </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B21">
+      <c r="S20" s="1"/>
+      <c r="T20" s="1"/>
+    </row>
+    <row r="21" spans="2:20" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="22">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F21" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="H21" s="9" t="s">
+      <c r="G21" s="23"/>
+      <c r="H21" s="23" t="s">
+        <v>295</v>
+      </c>
+      <c r="I21" s="23" t="s">
         <v>258</v>
       </c>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
-      <c r="P21" s="1"/>
-      <c r="Q21" s="1"/>
-      <c r="R21" s="1"/>
-    </row>
-    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B22">
+      <c r="J21" s="23" t="s">
+        <v>302</v>
+      </c>
+      <c r="K21" s="23"/>
+      <c r="L21" s="23"/>
+      <c r="M21" s="23"/>
+      <c r="N21" s="23"/>
+      <c r="O21" s="23"/>
+      <c r="P21" s="23"/>
+      <c r="Q21" s="23"/>
+      <c r="R21" s="23"/>
+      <c r="S21" s="23"/>
+      <c r="T21" s="23"/>
+    </row>
+    <row r="22" spans="2:20" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="22">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E22" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F22" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="G22" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="H22" s="9" t="s">
+      <c r="H22" s="23" t="s">
+        <v>295</v>
+      </c>
+      <c r="I22" s="23" t="s">
         <v>259</v>
       </c>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="1"/>
-      <c r="O22" s="1"/>
-      <c r="P22" s="1"/>
-      <c r="Q22" s="1"/>
-      <c r="R22" s="1"/>
-    </row>
-    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B23">
+      <c r="J22" s="23" t="s">
+        <v>302</v>
+      </c>
+      <c r="K22" s="23"/>
+      <c r="L22" s="23"/>
+      <c r="M22" s="23"/>
+      <c r="N22" s="23"/>
+      <c r="O22" s="23"/>
+      <c r="P22" s="23"/>
+      <c r="Q22" s="23"/>
+      <c r="R22" s="23"/>
+      <c r="S22" s="23"/>
+      <c r="T22" s="23"/>
+    </row>
+    <row r="23" spans="2:20" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="22">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E23" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="F23" s="9" t="s">
+      <c r="F23" s="23" t="s">
         <v>274</v>
       </c>
-      <c r="H23" s="9" t="s">
+      <c r="G23" s="23"/>
+      <c r="H23" s="23" t="s">
+        <v>295</v>
+      </c>
+      <c r="I23" s="23" t="s">
         <v>260</v>
       </c>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
-      <c r="O23" s="1"/>
-      <c r="P23" s="1"/>
-      <c r="Q23" s="1"/>
-      <c r="R23" s="1"/>
-    </row>
-    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B24">
+      <c r="J23" s="23" t="s">
+        <v>302</v>
+      </c>
+      <c r="K23" s="23"/>
+      <c r="L23" s="23"/>
+      <c r="M23" s="23"/>
+      <c r="N23" s="23"/>
+      <c r="O23" s="23"/>
+      <c r="P23" s="23"/>
+      <c r="Q23" s="23"/>
+      <c r="R23" s="23"/>
+      <c r="S23" s="23"/>
+      <c r="T23" s="23"/>
+    </row>
+    <row r="24" spans="2:20" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="22">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="F24" s="9" t="s">
+      <c r="F24" s="23" t="s">
         <v>275</v>
       </c>
-      <c r="H24" s="9" t="s">
+      <c r="G24" s="23"/>
+      <c r="H24" s="23" t="s">
+        <v>295</v>
+      </c>
+      <c r="I24" s="23" t="s">
         <v>261</v>
       </c>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="1"/>
-      <c r="O24" s="1"/>
-      <c r="P24" s="1"/>
-      <c r="Q24" s="1"/>
-      <c r="R24" s="1"/>
-    </row>
-    <row r="25" spans="2:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="J24" s="23" t="s">
+        <v>302</v>
+      </c>
+      <c r="K24" s="23"/>
+      <c r="L24" s="23"/>
+      <c r="M24" s="23"/>
+      <c r="N24" s="23"/>
+      <c r="O24" s="23"/>
+      <c r="P24" s="23"/>
+      <c r="Q24" s="23"/>
+      <c r="R24" s="23"/>
+      <c r="S24" s="23"/>
+      <c r="T24" s="23"/>
+    </row>
+    <row r="25" spans="2:20" ht="30" x14ac:dyDescent="0.25">
       <c r="B25">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -2708,11 +2844,12 @@
       <c r="G25" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H25" s="9" t="s">
+      <c r="I25" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
+      <c r="J25" s="9" t="s">
+        <v>303</v>
+      </c>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
@@ -2721,8 +2858,10 @@
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
-    </row>
-    <row r="26" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="S25" s="1"/>
+      <c r="T25" s="1"/>
+    </row>
+    <row r="26" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B26">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -2742,11 +2881,12 @@
       <c r="G26" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H26" s="9" t="s">
+      <c r="I26" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
+      <c r="J26" s="9" t="s">
+        <v>303</v>
+      </c>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
@@ -2755,109 +2895,125 @@
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
-    </row>
-    <row r="27" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B27">
+      <c r="S26" s="1"/>
+      <c r="T26" s="1"/>
+    </row>
+    <row r="27" spans="2:20" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="22">
         <f>B26+1</f>
         <v>23</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" s="23" t="s">
         <v>242</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D27" s="23" t="s">
         <v>243</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E27" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="F27" s="23" t="s">
         <v>244</v>
       </c>
-      <c r="H27" s="9" t="s">
+      <c r="G27" s="23"/>
+      <c r="H27" s="23"/>
+      <c r="I27" s="23" t="s">
         <v>262</v>
       </c>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
-      <c r="L27" s="1"/>
-      <c r="M27" s="1"/>
-      <c r="N27" s="1"/>
-      <c r="O27" s="1"/>
-      <c r="P27" s="1"/>
-      <c r="Q27" s="1"/>
-      <c r="R27" s="1"/>
-    </row>
-    <row r="28" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B28">
+      <c r="J27" s="23" t="s">
+        <v>302</v>
+      </c>
+      <c r="K27" s="23"/>
+      <c r="L27" s="23"/>
+      <c r="M27" s="23"/>
+      <c r="N27" s="23"/>
+      <c r="O27" s="23"/>
+      <c r="P27" s="23"/>
+      <c r="Q27" s="23"/>
+      <c r="R27" s="23"/>
+      <c r="S27" s="23"/>
+      <c r="T27" s="23"/>
+    </row>
+    <row r="28" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B28" s="22">
         <f>B26+1</f>
         <v>23</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D28" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E28" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="F28" s="23" t="s">
         <v>241</v>
       </c>
-      <c r="G28" s="1" t="s">
+      <c r="G28" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="H28" s="9" t="s">
+      <c r="H28" s="23"/>
+      <c r="I28" s="23" t="s">
         <v>263</v>
       </c>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
-      <c r="M28" s="1"/>
-      <c r="N28" s="1"/>
-      <c r="O28" s="1"/>
-      <c r="P28" s="1"/>
-      <c r="Q28" s="1"/>
-      <c r="R28" s="1"/>
-    </row>
-    <row r="29" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B29">
+      <c r="J28" s="23" t="s">
+        <v>302</v>
+      </c>
+      <c r="K28" s="23"/>
+      <c r="L28" s="23"/>
+      <c r="M28" s="23"/>
+      <c r="N28" s="23"/>
+      <c r="O28" s="23"/>
+      <c r="P28" s="23"/>
+      <c r="Q28" s="23"/>
+      <c r="R28" s="23"/>
+      <c r="S28" s="23"/>
+      <c r="T28" s="23"/>
+    </row>
+    <row r="29" spans="2:20" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="22">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D29" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E29" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="F29" s="23" t="s">
         <v>241</v>
       </c>
-      <c r="H29" s="9" t="s">
+      <c r="G29" s="23"/>
+      <c r="H29" s="23"/>
+      <c r="I29" s="23" t="s">
         <v>264</v>
       </c>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
-      <c r="L29" s="1"/>
-      <c r="M29" s="1"/>
-      <c r="N29" s="1"/>
-      <c r="O29" s="1"/>
-      <c r="P29" s="1"/>
-      <c r="Q29" s="1"/>
-      <c r="R29" s="1"/>
-    </row>
-    <row r="31" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="J29" s="23" t="s">
+        <v>302</v>
+      </c>
+      <c r="K29" s="23"/>
+      <c r="L29" s="23"/>
+      <c r="M29" s="23"/>
+      <c r="N29" s="23"/>
+      <c r="O29" s="23"/>
+      <c r="P29" s="23"/>
+      <c r="Q29" s="23"/>
+      <c r="R29" s="23"/>
+      <c r="S29" s="23"/>
+      <c r="T29" s="23"/>
+    </row>
+    <row r="31" spans="2:20" x14ac:dyDescent="0.25">
       <c r="F31" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="32" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:20" x14ac:dyDescent="0.25">
       <c r="F32" s="1" t="s">
         <v>97</v>
       </c>
@@ -2889,7 +3045,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="J2:X2"/>
+    <mergeCell ref="L2:Z2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3120,8 +3276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A3:L27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3131,7 +3287,7 @@
     <col min="4" max="4" width="10" style="1" customWidth="1"/>
     <col min="5" max="5" width="27.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.85546875" style="1"/>
-    <col min="7" max="7" width="21.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="31.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -3198,40 +3354,40 @@
     </row>
     <row r="6" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="23" t="s">
         <v>160</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="23" t="s">
         <v>161</v>
       </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9" t="s">
+      <c r="F6" s="23"/>
+      <c r="G6" s="23" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="7" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="23" t="s">
         <v>163</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="23" t="s">
         <v>161</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="23" t="s">
         <v>267</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Continued work on EX stage
</commit_message>
<xml_diff>
--- a/IS.xlsx
+++ b/IS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Okasha\Documents\modifiedMIPS\modifiedMIPS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6F6A9C1-EDD9-46FE-8377-96823AFDD8E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{188A749B-FA01-4F44-A0F6-7089E69B2F96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3405" windowWidth="11970" windowHeight="10200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3405" windowWidth="11970" windowHeight="10200" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instr. Formats" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="307">
   <si>
     <t>FORMAT</t>
   </si>
@@ -945,13 +945,22 @@
     <t>000100</t>
   </si>
   <si>
-    <t>ALU OPc</t>
-  </si>
-  <si>
     <t>010</t>
   </si>
   <si>
     <t>000</t>
+  </si>
+  <si>
+    <t>ALU Opc</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>ALUop</t>
   </si>
 </sst>
 </file>
@@ -990,7 +999,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1024,6 +1033,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1092,7 +1107,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1123,6 +1138,8 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1141,24 +1158,196 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="32">
+  <dxfs count="34">
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <fill>
-        <patternFill patternType="solid">
+        <patternFill patternType="none">
           <fgColor indexed="64"/>
-          <bgColor rgb="FF92D050"/>
+          <bgColor rgb="FFC00000"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -1206,60 +1395,6 @@
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1274,57 +1409,57 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="B3:T29" totalsRowShown="0" headerRowDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="B3:T29" totalsRowShown="0" headerRowDxfId="33" dataDxfId="3">
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="No.">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="No." dataDxfId="19">
       <calculatedColumnFormula>B3+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="NAME" dataDxfId="30"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="MNEMONIC" dataDxfId="29"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="FORMAT" dataDxfId="28"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="OPERATION (in Verilog)" dataDxfId="27"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Note" dataDxfId="26"/>
-    <tableColumn id="18" xr3:uid="{DFACAFC1-11FF-491F-9AB8-4002EB4348F8}" name="OPCODE zay el kheleg" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="OPCODE/ FUNCT(Hex)" dataDxfId="25"/>
-    <tableColumn id="19" xr3:uid="{7A4C5E34-6C04-4A0B-87EB-FBF54DC3C353}" name="ALU OPc" dataDxfId="0"/>
-    <tableColumn id="8" xr3:uid="{EE7F7B4D-DDD2-489C-8627-F67632B6806B}" name="ALU OP" dataDxfId="24"/>
-    <tableColumn id="9" xr3:uid="{AAFC0202-CB70-4B1A-9AF4-7E75B12C923B}" name="MemWrite" dataDxfId="23"/>
-    <tableColumn id="10" xr3:uid="{D4CA723B-8BCB-47DF-81D6-CE8E45FA7F18}" name="RegWrite" dataDxfId="22"/>
-    <tableColumn id="11" xr3:uid="{F06965CD-61B4-44BE-AFFB-16FD9D4BB004}" name="ALUs" dataDxfId="21"/>
-    <tableColumn id="12" xr3:uid="{BAC6153E-232C-4723-973E-5135B68C73F1}" name="Float" dataDxfId="20"/>
-    <tableColumn id="13" xr3:uid="{9E280564-ACAE-4469-8DE1-F31D0FCA6F71}" name="RegDst" dataDxfId="19"/>
-    <tableColumn id="14" xr3:uid="{856F9B53-AECE-404A-BB0B-7759D6599868}" name="HiLoWrite" dataDxfId="18"/>
-    <tableColumn id="15" xr3:uid="{C2001F97-A3F7-4884-9E5D-BC4ACC8AE232}" name="HL" dataDxfId="17"/>
-    <tableColumn id="16" xr3:uid="{8BA1CFC8-404A-4666-B7C9-97101DA879B4}" name="WBSrc" dataDxfId="16"/>
-    <tableColumn id="17" xr3:uid="{69D73963-7CBA-4A8D-8D02-94AC9142117F}" name="ALUc" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="NAME" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="MNEMONIC" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="FORMAT" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="OPERATION (in Verilog)" dataDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Note" dataDxfId="14"/>
+    <tableColumn id="18" xr3:uid="{DFACAFC1-11FF-491F-9AB8-4002EB4348F8}" name="OPCODE zay el kheleg" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="OPCODE/ FUNCT(Hex)" dataDxfId="2"/>
+    <tableColumn id="19" xr3:uid="{7A4C5E34-6C04-4A0B-87EB-FBF54DC3C353}" name="ALU Opc" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{EE7F7B4D-DDD2-489C-8627-F67632B6806B}" name="ALU OP" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{AAFC0202-CB70-4B1A-9AF4-7E75B12C923B}" name="MemWrite" dataDxfId="12"/>
+    <tableColumn id="10" xr3:uid="{D4CA723B-8BCB-47DF-81D6-CE8E45FA7F18}" name="RegWrite" dataDxfId="11"/>
+    <tableColumn id="11" xr3:uid="{F06965CD-61B4-44BE-AFFB-16FD9D4BB004}" name="ALUs" dataDxfId="10"/>
+    <tableColumn id="12" xr3:uid="{BAC6153E-232C-4723-973E-5135B68C73F1}" name="Float" dataDxfId="9"/>
+    <tableColumn id="13" xr3:uid="{9E280564-ACAE-4469-8DE1-F31D0FCA6F71}" name="RegDst" dataDxfId="8"/>
+    <tableColumn id="14" xr3:uid="{856F9B53-AECE-404A-BB0B-7759D6599868}" name="HiLoWrite" dataDxfId="7"/>
+    <tableColumn id="15" xr3:uid="{C2001F97-A3F7-4884-9E5D-BC4ACC8AE232}" name="HL" dataDxfId="6"/>
+    <tableColumn id="16" xr3:uid="{8BA1CFC8-404A-4666-B7C9-97101DA879B4}" name="WBSrc" dataDxfId="5"/>
+    <tableColumn id="17" xr3:uid="{69D73963-7CBA-4A8D-8D02-94AC9142117F}" name="ALUc" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="B3:E14" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="B3:E14" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
   <autoFilter ref="B3:E14" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="NAME" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="NUMBER" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="USE" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="PRESERVED ACROSS A CALL?" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="NAME" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="NUMBER" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="USE" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="PRESERVED ACROSS A CALL?" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table3" displayName="Table3" ref="B3:G27" totalsRowShown="0" headerRowDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table3" displayName="Table3" ref="B3:G27" totalsRowShown="0" headerRowDxfId="26">
   <autoFilter ref="B3:G27" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="NAME" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="MNEMONIC" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="FORMAT" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="OPERATION" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Note" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Opcode/ FMT /FT/ FUNCT(Hex)" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="NAME" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="MNEMONIC" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="FORMAT" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="OPERATION" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Note" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Opcode/ FMT /FT/ FUNCT(Hex)" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1613,30 +1748,30 @@
       <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16" t="s">
+      <c r="D5" s="18"/>
+      <c r="E5" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16" t="s">
+      <c r="F5" s="18"/>
+      <c r="G5" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16" t="s">
+      <c r="H5" s="18"/>
+      <c r="I5" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16" t="s">
+      <c r="J5" s="18"/>
+      <c r="K5" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="L5" s="16"/>
-      <c r="M5" s="16" t="s">
+      <c r="L5" s="18"/>
+      <c r="M5" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="N5" s="16"/>
+      <c r="N5" s="18"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C6" s="4">
@@ -1680,26 +1815,26 @@
       <c r="B8" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16" t="s">
+      <c r="D8" s="18"/>
+      <c r="E8" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16" t="s">
+      <c r="F8" s="18"/>
+      <c r="G8" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="H8" s="16"/>
-      <c r="I8" s="17" t="s">
+      <c r="H8" s="18"/>
+      <c r="I8" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="19"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="21"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C9" s="4">
@@ -1735,22 +1870,22 @@
       <c r="B11" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="D11" s="16"/>
-      <c r="E11" s="17" t="s">
+      <c r="D11" s="18"/>
+      <c r="E11" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="18"/>
-      <c r="M11" s="18"/>
-      <c r="N11" s="19"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="21"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C12" s="4">
@@ -1778,30 +1913,30 @@
       <c r="B16" t="s">
         <v>166</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16" t="s">
+      <c r="D16" s="18"/>
+      <c r="E16" s="18" t="s">
         <v>233</v>
       </c>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16" t="s">
+      <c r="F16" s="18"/>
+      <c r="G16" s="18" t="s">
         <v>234</v>
       </c>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16" t="s">
+      <c r="H16" s="18"/>
+      <c r="I16" s="18" t="s">
         <v>235</v>
       </c>
-      <c r="J16" s="16"/>
-      <c r="K16" s="16" t="s">
+      <c r="J16" s="18"/>
+      <c r="K16" s="18" t="s">
         <v>236</v>
       </c>
-      <c r="L16" s="16"/>
-      <c r="M16" s="16" t="s">
+      <c r="L16" s="18"/>
+      <c r="M16" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="N16" s="16"/>
+      <c r="N16" s="18"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C17" s="4">
@@ -1845,26 +1980,26 @@
       <c r="B19" t="s">
         <v>152</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16" t="s">
+      <c r="D19" s="18"/>
+      <c r="E19" s="18" t="s">
         <v>233</v>
       </c>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16" t="s">
+      <c r="F19" s="18"/>
+      <c r="G19" s="18" t="s">
         <v>234</v>
       </c>
-      <c r="H19" s="16"/>
-      <c r="I19" s="17" t="s">
+      <c r="H19" s="18"/>
+      <c r="I19" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="J19" s="18"/>
-      <c r="K19" s="18"/>
-      <c r="L19" s="18"/>
-      <c r="M19" s="18"/>
-      <c r="N19" s="19"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
+      <c r="M19" s="20"/>
+      <c r="N19" s="21"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C20" s="4">
@@ -1898,6 +2033,18 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:N11"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="I8:N8"/>
     <mergeCell ref="M16:N16"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="E19:F19"/>
@@ -1908,18 +2055,6 @@
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="I16:J16"/>
     <mergeCell ref="K16:L16"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:N11"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="I8:N8"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1929,8 +2064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:Z37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1942,28 +2077,28 @@
     <col min="7" max="7" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.28515625" style="1" customWidth="1"/>
     <col min="9" max="9" width="29" style="9" customWidth="1"/>
-    <col min="10" max="10" width="9.85546875" style="9" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" style="26" customWidth="1"/>
     <col min="12" max="12" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="L2" s="20" t="s">
+      <c r="L2" s="22" t="s">
         <v>281</v>
       </c>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="20"/>
-      <c r="S2" s="20"/>
-      <c r="T2" s="20"/>
-      <c r="U2" s="20"/>
-      <c r="V2" s="20"/>
-      <c r="W2" s="20"/>
-      <c r="X2" s="20"/>
-      <c r="Y2" s="20"/>
-      <c r="Z2" s="20"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="22"/>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="22"/>
+      <c r="S2" s="22"/>
+      <c r="T2" s="22"/>
+      <c r="U2" s="22"/>
+      <c r="V2" s="22"/>
+      <c r="W2" s="22"/>
+      <c r="X2" s="22"/>
+      <c r="Y2" s="22"/>
+      <c r="Z2" s="22"/>
     </row>
     <row r="3" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -1990,8 +2125,8 @@
       <c r="I3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="9" t="s">
-        <v>301</v>
+      <c r="J3" s="27" t="s">
+        <v>303</v>
       </c>
       <c r="K3" s="14" t="s">
         <v>276</v>
@@ -2024,989 +2159,1026 @@
         <v>290</v>
       </c>
     </row>
-    <row r="4" spans="2:26" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="22">
+    <row r="4" spans="2:26" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="16">
         <v>1</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="E4" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="23" t="s">
+      <c r="F4" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="23" t="s">
+      <c r="G4" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="23" t="s">
+      <c r="H4" s="17" t="s">
         <v>295</v>
       </c>
-      <c r="I4" s="23" t="s">
+      <c r="I4" s="17" t="s">
         <v>252</v>
       </c>
-      <c r="J4" s="23" t="s">
-        <v>302</v>
-      </c>
-      <c r="K4" s="23" t="s">
+      <c r="J4" s="26" t="s">
+        <v>301</v>
+      </c>
+      <c r="K4" s="17" t="s">
         <v>277</v>
       </c>
-      <c r="L4" s="23" t="s">
+      <c r="L4" s="17" t="s">
         <v>291</v>
       </c>
-      <c r="M4" s="23" t="s">
+      <c r="M4" s="17" t="s">
         <v>292</v>
       </c>
-      <c r="N4" s="23" t="s">
+      <c r="N4" s="17" t="s">
         <v>291</v>
       </c>
-      <c r="O4" s="23" t="s">
+      <c r="O4" s="17" t="s">
         <v>291</v>
       </c>
-      <c r="P4" s="23" t="s">
+      <c r="P4" s="17" t="s">
         <v>291</v>
       </c>
-      <c r="Q4" s="23" t="s">
+      <c r="Q4" s="17" t="s">
         <v>291</v>
       </c>
-      <c r="R4" s="23" t="s">
+      <c r="R4" s="17" t="s">
         <v>293</v>
       </c>
-      <c r="S4" s="23" t="s">
+      <c r="S4" s="17" t="s">
         <v>291</v>
       </c>
-      <c r="T4" s="23"/>
-    </row>
-    <row r="5" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B5">
+      <c r="T4" s="17"/>
+    </row>
+    <row r="5" spans="2:26" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="16">
         <f>B4+1</f>
         <v>2</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="17" t="s">
         <v>296</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="I5" s="17" t="s">
         <v>240</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="J5" s="26" t="s">
+        <v>302</v>
+      </c>
+      <c r="K5" s="17" t="s">
         <v>277</v>
       </c>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
-      <c r="S5" s="1"/>
-      <c r="T5" s="1"/>
-    </row>
-    <row r="6" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B6">
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17"/>
+      <c r="O5" s="17"/>
+      <c r="P5" s="17"/>
+      <c r="Q5" s="17"/>
+      <c r="R5" s="17"/>
+      <c r="S5" s="17"/>
+      <c r="T5" s="17"/>
+    </row>
+    <row r="6" spans="2:26" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="12">
         <f t="shared" ref="B6:B29" si="0">B5+1</f>
         <v>3</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="25" t="s">
         <v>297</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="I6" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="J6" s="26" t="s">
+        <v>302</v>
+      </c>
+      <c r="K6" s="25" t="s">
         <v>277</v>
       </c>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
-      <c r="R6" s="1"/>
-      <c r="S6" s="1"/>
-      <c r="T6" s="1"/>
-    </row>
-    <row r="7" spans="2:26" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="22">
+      <c r="L6" s="25"/>
+      <c r="M6" s="25"/>
+      <c r="N6" s="25"/>
+      <c r="O6" s="25"/>
+      <c r="P6" s="25"/>
+      <c r="Q6" s="25"/>
+      <c r="R6" s="25"/>
+      <c r="S6" s="25"/>
+      <c r="T6" s="25"/>
+    </row>
+    <row r="7" spans="2:26" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="16">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="D7" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="23" t="s">
+      <c r="E7" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="23" t="s">
+      <c r="F7" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23" t="s">
+      <c r="G7" s="17"/>
+      <c r="H7" s="17" t="s">
         <v>295</v>
       </c>
-      <c r="I7" s="23" t="s">
+      <c r="I7" s="17" t="s">
         <v>253</v>
       </c>
-      <c r="J7" s="23" t="s">
-        <v>302</v>
-      </c>
-      <c r="K7" s="23" t="s">
+      <c r="J7" s="26" t="s">
+        <v>301</v>
+      </c>
+      <c r="K7" s="17" t="s">
         <v>278</v>
       </c>
-      <c r="L7" s="23"/>
-      <c r="M7" s="23"/>
-      <c r="N7" s="23"/>
-      <c r="O7" s="23"/>
-      <c r="P7" s="23"/>
-      <c r="Q7" s="23"/>
-      <c r="R7" s="23"/>
-      <c r="S7" s="23"/>
-      <c r="T7" s="23"/>
-    </row>
-    <row r="8" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B8">
+      <c r="L7" s="17"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="17"/>
+      <c r="O7" s="17"/>
+      <c r="P7" s="17"/>
+      <c r="Q7" s="17"/>
+      <c r="R7" s="17"/>
+      <c r="S7" s="17"/>
+      <c r="T7" s="17"/>
+    </row>
+    <row r="8" spans="2:26" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="16">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="17" t="s">
         <v>298</v>
       </c>
-      <c r="I8" s="9" t="s">
+      <c r="I8" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="J8" s="17" t="s">
+        <v>305</v>
+      </c>
+      <c r="K8" s="17" t="s">
         <v>278</v>
       </c>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
-      <c r="R8" s="1"/>
-      <c r="S8" s="1"/>
-      <c r="T8" s="1"/>
-    </row>
-    <row r="9" spans="2:26" ht="30" x14ac:dyDescent="0.25">
-      <c r="B9">
+      <c r="L8" s="17"/>
+      <c r="M8" s="17"/>
+      <c r="N8" s="17"/>
+      <c r="O8" s="17"/>
+      <c r="P8" s="17"/>
+      <c r="Q8" s="17"/>
+      <c r="R8" s="17"/>
+      <c r="S8" s="17"/>
+      <c r="T8" s="17"/>
+    </row>
+    <row r="9" spans="2:26" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B9" s="16">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="17" t="s">
         <v>299</v>
       </c>
-      <c r="I9" s="9" t="s">
+      <c r="I9" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="J9" s="26" t="s">
+        <v>304</v>
+      </c>
+      <c r="K9" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="1"/>
-      <c r="S9" s="1"/>
-      <c r="T9" s="1"/>
-    </row>
-    <row r="10" spans="2:26" ht="30" x14ac:dyDescent="0.25">
-      <c r="B10">
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="17"/>
+      <c r="P9" s="17"/>
+      <c r="Q9" s="17"/>
+      <c r="R9" s="17"/>
+      <c r="S9" s="17"/>
+      <c r="T9" s="17"/>
+    </row>
+    <row r="10" spans="2:26" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B10" s="16">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H10" s="17" t="s">
         <v>300</v>
       </c>
-      <c r="I10" s="9" t="s">
+      <c r="I10" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="J10" s="26" t="s">
+        <v>304</v>
+      </c>
+      <c r="K10" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
-      <c r="S10" s="1"/>
-      <c r="T10" s="1"/>
-    </row>
-    <row r="11" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B11">
+      <c r="L10" s="17"/>
+      <c r="M10" s="17"/>
+      <c r="N10" s="17"/>
+      <c r="O10" s="17"/>
+      <c r="P10" s="17"/>
+      <c r="Q10" s="17"/>
+      <c r="R10" s="17"/>
+      <c r="S10" s="17"/>
+      <c r="T10" s="17"/>
+    </row>
+    <row r="11" spans="2:26" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="10">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G11" s="9" t="s">
         <v>45</v>
       </c>
+      <c r="H11" s="9"/>
       <c r="I11" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
-      <c r="R11" s="1"/>
-      <c r="S11" s="1"/>
-      <c r="T11" s="1"/>
-    </row>
-    <row r="12" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B12">
+      <c r="J11" s="26"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="9"/>
+      <c r="T11" s="9"/>
+    </row>
+    <row r="12" spans="2:26" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="10">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" s="9" t="s">
         <v>280</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G12" s="9" t="s">
         <v>45</v>
       </c>
+      <c r="H12" s="9"/>
       <c r="I12" s="9" t="s">
         <v>265</v>
       </c>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
-      <c r="Q12" s="1"/>
-      <c r="R12" s="1"/>
-      <c r="S12" s="1"/>
-      <c r="T12" s="1"/>
-    </row>
-    <row r="13" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B13">
+      <c r="J12" s="26"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="9"/>
+      <c r="S12" s="9"/>
+      <c r="T12" s="9"/>
+    </row>
+    <row r="13" spans="2:26" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="10">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="9" t="s">
         <v>11</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>273</v>
       </c>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
       <c r="I13" s="9" t="s">
         <v>254</v>
       </c>
-      <c r="K13" s="1" t="s">
+      <c r="J13" s="26"/>
+      <c r="K13" s="9" t="s">
         <v>277</v>
       </c>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
-      <c r="Q13" s="1"/>
-      <c r="R13" s="1"/>
-      <c r="S13" s="1"/>
-      <c r="T13" s="1"/>
-    </row>
-    <row r="14" spans="2:26" ht="30" x14ac:dyDescent="0.25">
-      <c r="B14">
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="9"/>
+      <c r="S13" s="9"/>
+      <c r="T13" s="9"/>
+    </row>
+    <row r="14" spans="2:26" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B14" s="16">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G14" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="I14" s="9" t="s">
+      <c r="H14" s="17"/>
+      <c r="I14" s="17" t="s">
         <v>237</v>
       </c>
-      <c r="K14" s="1" t="s">
+      <c r="J14" s="26" t="s">
+        <v>302</v>
+      </c>
+      <c r="K14" s="17" t="s">
         <v>277</v>
       </c>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
-      <c r="Q14" s="1"/>
-      <c r="R14" s="1"/>
-      <c r="S14" s="1"/>
-      <c r="T14" s="1"/>
-    </row>
-    <row r="15" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B15">
+      <c r="L14" s="17"/>
+      <c r="M14" s="17"/>
+      <c r="N14" s="17"/>
+      <c r="O14" s="17"/>
+      <c r="P14" s="17"/>
+      <c r="Q14" s="17"/>
+      <c r="R14" s="17"/>
+      <c r="S14" s="17"/>
+      <c r="T14" s="17"/>
+    </row>
+    <row r="15" spans="2:26" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="16">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F15" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="I15" s="9" t="s">
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
-      <c r="Q15" s="1"/>
-      <c r="R15" s="1"/>
-      <c r="S15" s="1"/>
-      <c r="T15" s="1"/>
-    </row>
-    <row r="16" spans="2:26" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="10">
+      <c r="J15" s="26" t="s">
+        <v>279</v>
+      </c>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="17"/>
+      <c r="N15" s="17"/>
+      <c r="O15" s="17"/>
+      <c r="P15" s="17"/>
+      <c r="Q15" s="17"/>
+      <c r="R15" s="17"/>
+      <c r="S15" s="17"/>
+      <c r="T15" s="17"/>
+    </row>
+    <row r="16" spans="2:26" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="16">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E16" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="F16" s="9" t="s">
+      <c r="F16" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="G16" s="9" t="s">
+      <c r="G16" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9" t="s">
+      <c r="H16" s="17"/>
+      <c r="I16" s="17" t="s">
         <v>238</v>
       </c>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9" t="s">
+      <c r="J16" s="26" t="s">
+        <v>302</v>
+      </c>
+      <c r="K16" s="17" t="s">
         <v>277</v>
       </c>
-      <c r="L16" s="9"/>
-      <c r="M16" s="9"/>
-      <c r="N16" s="9"/>
-      <c r="O16" s="9"/>
-      <c r="P16" s="9"/>
-      <c r="Q16" s="9"/>
-      <c r="R16" s="9"/>
-      <c r="S16" s="9"/>
-      <c r="T16" s="9"/>
-    </row>
-    <row r="17" spans="2:20" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="22">
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="17"/>
+      <c r="O16" s="17"/>
+      <c r="P16" s="17"/>
+      <c r="Q16" s="17"/>
+      <c r="R16" s="17"/>
+      <c r="S16" s="17"/>
+      <c r="T16" s="17"/>
+    </row>
+    <row r="17" spans="2:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="16">
         <f>B16+1</f>
         <v>14</v>
       </c>
-      <c r="C17" s="23" t="s">
+      <c r="C17" s="17" t="s">
         <v>245</v>
       </c>
-      <c r="D17" s="23" t="s">
+      <c r="D17" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="E17" s="23" t="s">
+      <c r="E17" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="23" t="s">
+      <c r="F17" s="17" t="s">
         <v>247</v>
       </c>
-      <c r="G17" s="23"/>
-      <c r="H17" s="23" t="s">
+      <c r="G17" s="17"/>
+      <c r="H17" s="17" t="s">
         <v>295</v>
       </c>
-      <c r="I17" s="23" t="s">
+      <c r="I17" s="17" t="s">
         <v>255</v>
       </c>
-      <c r="J17" s="23" t="s">
-        <v>302</v>
-      </c>
-      <c r="K17" s="23"/>
-      <c r="L17" s="23"/>
-      <c r="M17" s="23"/>
-      <c r="N17" s="23"/>
-      <c r="O17" s="23"/>
-      <c r="P17" s="23"/>
-      <c r="Q17" s="23"/>
-      <c r="R17" s="23"/>
-      <c r="S17" s="23"/>
-      <c r="T17" s="23"/>
-    </row>
-    <row r="18" spans="2:20" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="22">
+      <c r="J17" s="26" t="s">
+        <v>301</v>
+      </c>
+      <c r="K17" s="17"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="17"/>
+      <c r="N17" s="17"/>
+      <c r="O17" s="17"/>
+      <c r="P17" s="17"/>
+      <c r="Q17" s="17"/>
+      <c r="R17" s="17"/>
+      <c r="S17" s="17"/>
+      <c r="T17" s="17"/>
+    </row>
+    <row r="18" spans="2:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="16">
         <f>B16+1</f>
         <v>14</v>
       </c>
-      <c r="C18" s="23" t="s">
+      <c r="C18" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="D18" s="23" t="s">
+      <c r="D18" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="E18" s="23" t="s">
+      <c r="E18" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="F18" s="23" t="s">
+      <c r="F18" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="G18" s="23"/>
-      <c r="H18" s="23" t="s">
+      <c r="G18" s="17"/>
+      <c r="H18" s="17" t="s">
         <v>295</v>
       </c>
-      <c r="I18" s="23" t="s">
+      <c r="I18" s="17" t="s">
         <v>256</v>
       </c>
-      <c r="J18" s="23" t="s">
-        <v>302</v>
-      </c>
-      <c r="K18" s="23"/>
-      <c r="L18" s="23"/>
-      <c r="M18" s="23"/>
-      <c r="N18" s="23"/>
-      <c r="O18" s="23"/>
-      <c r="P18" s="23"/>
-      <c r="Q18" s="23"/>
-      <c r="R18" s="23"/>
-      <c r="S18" s="23"/>
-      <c r="T18" s="23"/>
-    </row>
-    <row r="19" spans="2:20" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="22">
+      <c r="J18" s="26" t="s">
+        <v>301</v>
+      </c>
+      <c r="K18" s="17"/>
+      <c r="L18" s="17"/>
+      <c r="M18" s="17"/>
+      <c r="N18" s="17"/>
+      <c r="O18" s="17"/>
+      <c r="P18" s="17"/>
+      <c r="Q18" s="17"/>
+      <c r="R18" s="17"/>
+      <c r="S18" s="17"/>
+      <c r="T18" s="17"/>
+    </row>
+    <row r="19" spans="2:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="16">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C19" s="23" t="s">
+      <c r="C19" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="D19" s="23" t="s">
+      <c r="D19" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="E19" s="23" t="s">
+      <c r="E19" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="F19" s="23" t="s">
+      <c r="F19" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="G19" s="23"/>
-      <c r="H19" s="23" t="s">
+      <c r="G19" s="17"/>
+      <c r="H19" s="17" t="s">
         <v>295</v>
       </c>
-      <c r="I19" s="23" t="s">
+      <c r="I19" s="17" t="s">
         <v>257</v>
       </c>
-      <c r="J19" s="23" t="s">
-        <v>302</v>
-      </c>
-      <c r="K19" s="23"/>
-      <c r="L19" s="23"/>
-      <c r="M19" s="23"/>
-      <c r="N19" s="23"/>
-      <c r="O19" s="23"/>
-      <c r="P19" s="23"/>
-      <c r="Q19" s="23"/>
-      <c r="R19" s="23"/>
-      <c r="S19" s="23"/>
-      <c r="T19" s="23"/>
-    </row>
-    <row r="20" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B20">
+      <c r="J19" s="26" t="s">
+        <v>301</v>
+      </c>
+      <c r="K19" s="17"/>
+      <c r="L19" s="17"/>
+      <c r="M19" s="17"/>
+      <c r="N19" s="17"/>
+      <c r="O19" s="17"/>
+      <c r="P19" s="17"/>
+      <c r="Q19" s="17"/>
+      <c r="R19" s="17"/>
+      <c r="S19" s="17"/>
+      <c r="T19" s="17"/>
+    </row>
+    <row r="20" spans="2:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="16">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F20" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="G20" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="I20" s="9" t="s">
+      <c r="H20" s="17"/>
+      <c r="I20" s="17" t="s">
         <v>239</v>
       </c>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
-      <c r="Q20" s="1"/>
-      <c r="R20" s="1"/>
-      <c r="S20" s="1"/>
-      <c r="T20" s="1"/>
-    </row>
-    <row r="21" spans="2:20" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="22">
+      <c r="J20" s="17"/>
+      <c r="K20" s="17"/>
+      <c r="L20" s="17"/>
+      <c r="M20" s="17"/>
+      <c r="N20" s="17"/>
+      <c r="O20" s="17"/>
+      <c r="P20" s="17"/>
+      <c r="Q20" s="17"/>
+      <c r="R20" s="17"/>
+      <c r="S20" s="17"/>
+      <c r="T20" s="17"/>
+    </row>
+    <row r="21" spans="2:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="16">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="C21" s="23" t="s">
+      <c r="C21" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="D21" s="23" t="s">
+      <c r="D21" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="E21" s="23" t="s">
+      <c r="E21" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="F21" s="23" t="s">
+      <c r="F21" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="G21" s="23"/>
-      <c r="H21" s="23" t="s">
+      <c r="G21" s="17"/>
+      <c r="H21" s="17" t="s">
         <v>295</v>
       </c>
-      <c r="I21" s="23" t="s">
+      <c r="I21" s="17" t="s">
         <v>258</v>
       </c>
-      <c r="J21" s="23" t="s">
-        <v>302</v>
-      </c>
-      <c r="K21" s="23"/>
-      <c r="L21" s="23"/>
-      <c r="M21" s="23"/>
-      <c r="N21" s="23"/>
-      <c r="O21" s="23"/>
-      <c r="P21" s="23"/>
-      <c r="Q21" s="23"/>
-      <c r="R21" s="23"/>
-      <c r="S21" s="23"/>
-      <c r="T21" s="23"/>
-    </row>
-    <row r="22" spans="2:20" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="22">
+      <c r="J21" s="26" t="s">
+        <v>301</v>
+      </c>
+      <c r="K21" s="17"/>
+      <c r="L21" s="17"/>
+      <c r="M21" s="17"/>
+      <c r="N21" s="17"/>
+      <c r="O21" s="17"/>
+      <c r="P21" s="17"/>
+      <c r="Q21" s="17"/>
+      <c r="R21" s="17"/>
+      <c r="S21" s="17"/>
+      <c r="T21" s="17"/>
+    </row>
+    <row r="22" spans="2:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="16">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="C22" s="23" t="s">
+      <c r="C22" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="D22" s="23" t="s">
+      <c r="D22" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="E22" s="23" t="s">
+      <c r="E22" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="F22" s="23" t="s">
+      <c r="F22" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="G22" s="23" t="s">
+      <c r="G22" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="H22" s="23" t="s">
+      <c r="H22" s="17" t="s">
         <v>295</v>
       </c>
-      <c r="I22" s="23" t="s">
+      <c r="I22" s="17" t="s">
         <v>259</v>
       </c>
-      <c r="J22" s="23" t="s">
-        <v>302</v>
-      </c>
-      <c r="K22" s="23"/>
-      <c r="L22" s="23"/>
-      <c r="M22" s="23"/>
-      <c r="N22" s="23"/>
-      <c r="O22" s="23"/>
-      <c r="P22" s="23"/>
-      <c r="Q22" s="23"/>
-      <c r="R22" s="23"/>
-      <c r="S22" s="23"/>
-      <c r="T22" s="23"/>
-    </row>
-    <row r="23" spans="2:20" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="22">
+      <c r="J22" s="26" t="s">
+        <v>301</v>
+      </c>
+      <c r="K22" s="17"/>
+      <c r="L22" s="17"/>
+      <c r="M22" s="17"/>
+      <c r="N22" s="17"/>
+      <c r="O22" s="17"/>
+      <c r="P22" s="17"/>
+      <c r="Q22" s="17"/>
+      <c r="R22" s="17"/>
+      <c r="S22" s="17"/>
+      <c r="T22" s="17"/>
+    </row>
+    <row r="23" spans="2:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="16">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="C23" s="23" t="s">
+      <c r="C23" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="D23" s="23" t="s">
+      <c r="D23" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="E23" s="23" t="s">
+      <c r="E23" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="F23" s="23" t="s">
+      <c r="F23" s="17" t="s">
         <v>274</v>
       </c>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23" t="s">
+      <c r="G23" s="17"/>
+      <c r="H23" s="17" t="s">
         <v>295</v>
       </c>
-      <c r="I23" s="23" t="s">
+      <c r="I23" s="17" t="s">
         <v>260</v>
       </c>
-      <c r="J23" s="23" t="s">
-        <v>302</v>
-      </c>
-      <c r="K23" s="23"/>
-      <c r="L23" s="23"/>
-      <c r="M23" s="23"/>
-      <c r="N23" s="23"/>
-      <c r="O23" s="23"/>
-      <c r="P23" s="23"/>
-      <c r="Q23" s="23"/>
-      <c r="R23" s="23"/>
-      <c r="S23" s="23"/>
-      <c r="T23" s="23"/>
-    </row>
-    <row r="24" spans="2:20" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="22">
+      <c r="J23" s="26" t="s">
+        <v>301</v>
+      </c>
+      <c r="K23" s="17"/>
+      <c r="L23" s="17"/>
+      <c r="M23" s="17"/>
+      <c r="N23" s="17"/>
+      <c r="O23" s="17"/>
+      <c r="P23" s="17"/>
+      <c r="Q23" s="17"/>
+      <c r="R23" s="17"/>
+      <c r="S23" s="17"/>
+      <c r="T23" s="17"/>
+    </row>
+    <row r="24" spans="2:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="16">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="C24" s="23" t="s">
+      <c r="C24" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="D24" s="23" t="s">
+      <c r="D24" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="E24" s="23" t="s">
+      <c r="E24" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="F24" s="23" t="s">
+      <c r="F24" s="17" t="s">
         <v>275</v>
       </c>
-      <c r="G24" s="23"/>
-      <c r="H24" s="23" t="s">
+      <c r="G24" s="17"/>
+      <c r="H24" s="17" t="s">
         <v>295</v>
       </c>
-      <c r="I24" s="23" t="s">
+      <c r="I24" s="17" t="s">
         <v>261</v>
       </c>
-      <c r="J24" s="23" t="s">
-        <v>302</v>
-      </c>
-      <c r="K24" s="23"/>
-      <c r="L24" s="23"/>
-      <c r="M24" s="23"/>
-      <c r="N24" s="23"/>
-      <c r="O24" s="23"/>
-      <c r="P24" s="23"/>
-      <c r="Q24" s="23"/>
-      <c r="R24" s="23"/>
-      <c r="S24" s="23"/>
-      <c r="T24" s="23"/>
-    </row>
-    <row r="25" spans="2:20" ht="30" x14ac:dyDescent="0.25">
-      <c r="B25">
+      <c r="J24" s="26" t="s">
+        <v>301</v>
+      </c>
+      <c r="K24" s="17"/>
+      <c r="L24" s="17"/>
+      <c r="M24" s="17"/>
+      <c r="N24" s="17"/>
+      <c r="O24" s="17"/>
+      <c r="P24" s="17"/>
+      <c r="Q24" s="17"/>
+      <c r="R24" s="17"/>
+      <c r="S24" s="17"/>
+      <c r="T24" s="17"/>
+    </row>
+    <row r="25" spans="2:20" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B25" s="16">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E25" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="F25" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="G25" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="I25" s="9" t="s">
+      <c r="H25" s="17"/>
+      <c r="I25" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="J25" s="9" t="s">
-        <v>303</v>
-      </c>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
-      <c r="O25" s="1"/>
-      <c r="P25" s="1"/>
-      <c r="Q25" s="1"/>
-      <c r="R25" s="1"/>
-      <c r="S25" s="1"/>
-      <c r="T25" s="1"/>
-    </row>
-    <row r="26" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B26">
+      <c r="J25" s="26" t="s">
+        <v>302</v>
+      </c>
+      <c r="K25" s="17"/>
+      <c r="L25" s="17"/>
+      <c r="M25" s="17"/>
+      <c r="N25" s="17"/>
+      <c r="O25" s="17"/>
+      <c r="P25" s="17"/>
+      <c r="Q25" s="17"/>
+      <c r="R25" s="17"/>
+      <c r="S25" s="17"/>
+      <c r="T25" s="17"/>
+    </row>
+    <row r="26" spans="2:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="16">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D26" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E26" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="F26" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="G26" s="1" t="s">
+      <c r="G26" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="I26" s="9" t="s">
+      <c r="H26" s="17"/>
+      <c r="I26" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="J26" s="9" t="s">
-        <v>303</v>
-      </c>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
-      <c r="N26" s="1"/>
-      <c r="O26" s="1"/>
-      <c r="P26" s="1"/>
-      <c r="Q26" s="1"/>
-      <c r="R26" s="1"/>
-      <c r="S26" s="1"/>
-      <c r="T26" s="1"/>
-    </row>
-    <row r="27" spans="2:20" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="22">
+      <c r="J26" s="26" t="s">
+        <v>302</v>
+      </c>
+      <c r="K26" s="17"/>
+      <c r="L26" s="17"/>
+      <c r="M26" s="17"/>
+      <c r="N26" s="17"/>
+      <c r="O26" s="17"/>
+      <c r="P26" s="17"/>
+      <c r="Q26" s="17"/>
+      <c r="R26" s="17"/>
+      <c r="S26" s="17"/>
+      <c r="T26" s="17"/>
+    </row>
+    <row r="27" spans="2:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="16">
         <f>B26+1</f>
         <v>23</v>
       </c>
-      <c r="C27" s="23" t="s">
+      <c r="C27" s="17" t="s">
         <v>242</v>
       </c>
-      <c r="D27" s="23" t="s">
+      <c r="D27" s="17" t="s">
         <v>243</v>
       </c>
-      <c r="E27" s="23" t="s">
+      <c r="E27" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="F27" s="23" t="s">
+      <c r="F27" s="17" t="s">
         <v>244</v>
       </c>
-      <c r="G27" s="23"/>
-      <c r="H27" s="23"/>
-      <c r="I27" s="23" t="s">
+      <c r="G27" s="17"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="17" t="s">
         <v>262</v>
       </c>
-      <c r="J27" s="23" t="s">
-        <v>302</v>
-      </c>
-      <c r="K27" s="23"/>
-      <c r="L27" s="23"/>
-      <c r="M27" s="23"/>
-      <c r="N27" s="23"/>
-      <c r="O27" s="23"/>
-      <c r="P27" s="23"/>
-      <c r="Q27" s="23"/>
-      <c r="R27" s="23"/>
-      <c r="S27" s="23"/>
-      <c r="T27" s="23"/>
-    </row>
-    <row r="28" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B28" s="22">
+      <c r="J27" s="26" t="s">
+        <v>301</v>
+      </c>
+      <c r="K27" s="17"/>
+      <c r="L27" s="17"/>
+      <c r="M27" s="17"/>
+      <c r="N27" s="17"/>
+      <c r="O27" s="17"/>
+      <c r="P27" s="17"/>
+      <c r="Q27" s="17"/>
+      <c r="R27" s="17"/>
+      <c r="S27" s="17"/>
+      <c r="T27" s="17"/>
+    </row>
+    <row r="28" spans="2:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="16">
         <f>B26+1</f>
         <v>23</v>
       </c>
-      <c r="C28" s="23" t="s">
+      <c r="C28" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="D28" s="23" t="s">
+      <c r="D28" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="E28" s="23" t="s">
+      <c r="E28" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="F28" s="23" t="s">
+      <c r="F28" s="17" t="s">
         <v>241</v>
       </c>
-      <c r="G28" s="23" t="s">
+      <c r="G28" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="H28" s="23"/>
-      <c r="I28" s="23" t="s">
+      <c r="H28" s="17"/>
+      <c r="I28" s="17" t="s">
         <v>263</v>
       </c>
-      <c r="J28" s="23" t="s">
-        <v>302</v>
-      </c>
-      <c r="K28" s="23"/>
-      <c r="L28" s="23"/>
-      <c r="M28" s="23"/>
-      <c r="N28" s="23"/>
-      <c r="O28" s="23"/>
-      <c r="P28" s="23"/>
-      <c r="Q28" s="23"/>
-      <c r="R28" s="23"/>
-      <c r="S28" s="23"/>
-      <c r="T28" s="23"/>
-    </row>
-    <row r="29" spans="2:20" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="22">
+      <c r="J28" s="26" t="s">
+        <v>301</v>
+      </c>
+      <c r="K28" s="17"/>
+      <c r="L28" s="17"/>
+      <c r="M28" s="17"/>
+      <c r="N28" s="17"/>
+      <c r="O28" s="17"/>
+      <c r="P28" s="17"/>
+      <c r="Q28" s="17"/>
+      <c r="R28" s="17"/>
+      <c r="S28" s="17"/>
+      <c r="T28" s="17"/>
+    </row>
+    <row r="29" spans="2:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="16">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="C29" s="23" t="s">
+      <c r="C29" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="D29" s="23" t="s">
+      <c r="D29" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="E29" s="23" t="s">
+      <c r="E29" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="F29" s="23" t="s">
+      <c r="F29" s="17" t="s">
         <v>241</v>
       </c>
-      <c r="G29" s="23"/>
-      <c r="H29" s="23"/>
-      <c r="I29" s="23" t="s">
+      <c r="G29" s="17"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="17" t="s">
         <v>264</v>
       </c>
-      <c r="J29" s="23" t="s">
-        <v>302</v>
-      </c>
-      <c r="K29" s="23"/>
-      <c r="L29" s="23"/>
-      <c r="M29" s="23"/>
-      <c r="N29" s="23"/>
-      <c r="O29" s="23"/>
-      <c r="P29" s="23"/>
-      <c r="Q29" s="23"/>
-      <c r="R29" s="23"/>
-      <c r="S29" s="23"/>
-      <c r="T29" s="23"/>
+      <c r="J29" s="26" t="s">
+        <v>301</v>
+      </c>
+      <c r="K29" s="17"/>
+      <c r="L29" s="17"/>
+      <c r="M29" s="17"/>
+      <c r="N29" s="17"/>
+      <c r="O29" s="17"/>
+      <c r="P29" s="17"/>
+      <c r="Q29" s="17"/>
+      <c r="R29" s="17"/>
+      <c r="S29" s="17"/>
+      <c r="T29" s="17"/>
     </row>
     <row r="31" spans="2:20" x14ac:dyDescent="0.25">
       <c r="F31" s="1" t="s">
@@ -3276,8 +3448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A3:L27"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3309,6 +3481,9 @@
       <c r="G3" s="1" t="s">
         <v>251</v>
       </c>
+      <c r="H3" t="s">
+        <v>306</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="12"/>
@@ -3330,6 +3505,7 @@
       <c r="G4" s="1" t="s">
         <v>154</v>
       </c>
+      <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
@@ -3351,44 +3527,51 @@
       <c r="G5" s="1" t="s">
         <v>158</v>
       </c>
+      <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="17" t="s">
         <v>159</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="17" t="s">
         <v>160</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="23" t="s">
+      <c r="E6" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23" t="s">
+      <c r="F6" s="17"/>
+      <c r="G6" s="17" t="s">
         <v>266</v>
       </c>
+      <c r="H6" s="9" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row r="7" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="17" t="s">
         <v>162</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="D7" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="23" t="s">
+      <c r="E7" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="F7" s="23" t="s">
+      <c r="F7" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="G7" s="23" t="s">
+      <c r="G7" s="17" t="s">
         <v>267</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="8" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -3409,6 +3592,7 @@
       <c r="G8" s="9" t="s">
         <v>168</v>
       </c>
+      <c r="H8" s="9"/>
     </row>
     <row r="9" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
@@ -3427,6 +3611,7 @@
       <c r="G9" s="1" t="s">
         <v>142</v>
       </c>
+      <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
@@ -3445,13 +3630,13 @@
       <c r="G10" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="H10" s="21" t="s">
+      <c r="H10" s="23" t="s">
         <v>144</v>
       </c>
-      <c r="I10" s="21"/>
-      <c r="J10" s="21"/>
-      <c r="K10" s="21"/>
-      <c r="L10" s="21"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="23"/>
     </row>
     <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
@@ -3470,11 +3655,11 @@
       <c r="G11" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="H11" s="21"/>
-      <c r="I11" s="21"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="21"/>
-      <c r="L11" s="21"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="23"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
@@ -3782,8 +3967,9 @@
     <mergeCell ref="H10:L11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added remaining instructions in ALU control Unit
</commit_message>
<xml_diff>
--- a/IS.xlsx
+++ b/IS.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Okasha\Documents\modifiedMIPS\modifiedMIPS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a.akasheh\Documents\Quartus\modifiedMIPS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{188A749B-FA01-4F44-A0F6-7089E69B2F96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3405" windowWidth="11970" windowHeight="10200" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3405" windowWidth="11970" windowHeight="10200" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Instr. Formats" sheetId="2" r:id="rId1"/>
@@ -18,7 +17,7 @@
     <sheet name="Registers" sheetId="3" r:id="rId3"/>
     <sheet name="Floating" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="307">
   <si>
     <t>FORMAT</t>
   </si>
@@ -966,7 +965,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -999,7 +998,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1009,12 +1008,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1107,7 +1100,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1137,9 +1130,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1152,19 +1152,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1173,38 +1165,46 @@
   <dxfs count="34">
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -1301,6 +1301,33 @@
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
           <bgColor auto="1"/>
         </patternFill>
       </fill>
@@ -1350,47 +1377,12 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -1409,57 +1401,57 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="B3:T29" totalsRowShown="0" headerRowDxfId="33" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B3:T29" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="No." dataDxfId="19">
+    <tableColumn id="1" name="No." dataDxfId="31">
       <calculatedColumnFormula>B3+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="NAME" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="MNEMONIC" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="FORMAT" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="OPERATION (in Verilog)" dataDxfId="15"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Note" dataDxfId="14"/>
-    <tableColumn id="18" xr3:uid="{DFACAFC1-11FF-491F-9AB8-4002EB4348F8}" name="OPCODE zay el kheleg" dataDxfId="13"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="OPCODE/ FUNCT(Hex)" dataDxfId="2"/>
-    <tableColumn id="19" xr3:uid="{7A4C5E34-6C04-4A0B-87EB-FBF54DC3C353}" name="ALU Opc" dataDxfId="0"/>
-    <tableColumn id="8" xr3:uid="{EE7F7B4D-DDD2-489C-8627-F67632B6806B}" name="ALU OP" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{AAFC0202-CB70-4B1A-9AF4-7E75B12C923B}" name="MemWrite" dataDxfId="12"/>
-    <tableColumn id="10" xr3:uid="{D4CA723B-8BCB-47DF-81D6-CE8E45FA7F18}" name="RegWrite" dataDxfId="11"/>
-    <tableColumn id="11" xr3:uid="{F06965CD-61B4-44BE-AFFB-16FD9D4BB004}" name="ALUs" dataDxfId="10"/>
-    <tableColumn id="12" xr3:uid="{BAC6153E-232C-4723-973E-5135B68C73F1}" name="Float" dataDxfId="9"/>
-    <tableColumn id="13" xr3:uid="{9E280564-ACAE-4469-8DE1-F31D0FCA6F71}" name="RegDst" dataDxfId="8"/>
-    <tableColumn id="14" xr3:uid="{856F9B53-AECE-404A-BB0B-7759D6599868}" name="HiLoWrite" dataDxfId="7"/>
-    <tableColumn id="15" xr3:uid="{C2001F97-A3F7-4884-9E5D-BC4ACC8AE232}" name="HL" dataDxfId="6"/>
-    <tableColumn id="16" xr3:uid="{8BA1CFC8-404A-4666-B7C9-97101DA879B4}" name="WBSrc" dataDxfId="5"/>
-    <tableColumn id="17" xr3:uid="{69D73963-7CBA-4A8D-8D02-94AC9142117F}" name="ALUc" dataDxfId="4"/>
+    <tableColumn id="2" name="NAME" dataDxfId="30"/>
+    <tableColumn id="3" name="MNEMONIC" dataDxfId="29"/>
+    <tableColumn id="4" name="FORMAT" dataDxfId="28"/>
+    <tableColumn id="5" name="OPERATION (in Verilog)" dataDxfId="27"/>
+    <tableColumn id="6" name="Note" dataDxfId="26"/>
+    <tableColumn id="18" name="OPCODE zay el kheleg" dataDxfId="25"/>
+    <tableColumn id="7" name="OPCODE/ FUNCT(Hex)" dataDxfId="24"/>
+    <tableColumn id="19" name="ALU Opc" dataDxfId="23"/>
+    <tableColumn id="8" name="ALU OP" dataDxfId="22"/>
+    <tableColumn id="9" name="MemWrite" dataDxfId="21"/>
+    <tableColumn id="10" name="RegWrite" dataDxfId="20"/>
+    <tableColumn id="11" name="ALUs" dataDxfId="19"/>
+    <tableColumn id="12" name="Float" dataDxfId="18"/>
+    <tableColumn id="13" name="RegDst" dataDxfId="17"/>
+    <tableColumn id="14" name="HiLoWrite" dataDxfId="16"/>
+    <tableColumn id="15" name="HL" dataDxfId="15"/>
+    <tableColumn id="16" name="WBSrc" dataDxfId="14"/>
+    <tableColumn id="17" name="ALUc" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="B3:E14" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
-  <autoFilter ref="B3:E14" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B3:E14" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="B3:E14"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="NAME" dataDxfId="30"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="NUMBER" dataDxfId="29"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="USE" dataDxfId="28"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="PRESERVED ACROSS A CALL?" dataDxfId="27"/>
+    <tableColumn id="1" name="NAME" dataDxfId="10"/>
+    <tableColumn id="2" name="NUMBER" dataDxfId="9"/>
+    <tableColumn id="3" name="USE" dataDxfId="8"/>
+    <tableColumn id="4" name="PRESERVED ACROSS A CALL?" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table3" displayName="Table3" ref="B3:G27" totalsRowShown="0" headerRowDxfId="26">
-  <autoFilter ref="B3:G27" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B3:G27" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="B3:G27"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="NAME" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="MNEMONIC" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="FORMAT" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="OPERATION" dataDxfId="22"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Note" dataDxfId="21"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Opcode/ FMT /FT/ FUNCT(Hex)" dataDxfId="20"/>
+    <tableColumn id="1" name="NAME" dataDxfId="5"/>
+    <tableColumn id="2" name="MNEMONIC" dataDxfId="4"/>
+    <tableColumn id="3" name="FORMAT" dataDxfId="3"/>
+    <tableColumn id="4" name="OPERATION" dataDxfId="2"/>
+    <tableColumn id="5" name="Note" dataDxfId="1"/>
+    <tableColumn id="6" name="Opcode/ FMT /FT/ FUNCT(Hex)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1727,7 +1719,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:N20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1748,30 +1740,30 @@
       <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18" t="s">
+      <c r="D5" s="21"/>
+      <c r="E5" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18" t="s">
+      <c r="F5" s="21"/>
+      <c r="G5" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18" t="s">
+      <c r="H5" s="21"/>
+      <c r="I5" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18" t="s">
+      <c r="J5" s="21"/>
+      <c r="K5" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="L5" s="18"/>
-      <c r="M5" s="18" t="s">
+      <c r="L5" s="21"/>
+      <c r="M5" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="N5" s="18"/>
+      <c r="N5" s="21"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C6" s="4">
@@ -1815,26 +1807,26 @@
       <c r="B8" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18" t="s">
+      <c r="D8" s="21"/>
+      <c r="E8" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18" t="s">
+      <c r="F8" s="21"/>
+      <c r="G8" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="H8" s="18"/>
-      <c r="I8" s="19" t="s">
+      <c r="H8" s="21"/>
+      <c r="I8" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20"/>
-      <c r="M8" s="20"/>
-      <c r="N8" s="21"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="24"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C9" s="4">
@@ -1870,22 +1862,22 @@
       <c r="B11" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="19" t="s">
+      <c r="D11" s="21"/>
+      <c r="E11" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="20"/>
-      <c r="M11" s="20"/>
-      <c r="N11" s="21"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="23"/>
+      <c r="N11" s="24"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C12" s="4">
@@ -1913,30 +1905,30 @@
       <c r="B16" t="s">
         <v>166</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18" t="s">
+      <c r="D16" s="21"/>
+      <c r="E16" s="21" t="s">
         <v>233</v>
       </c>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18" t="s">
+      <c r="F16" s="21"/>
+      <c r="G16" s="21" t="s">
         <v>234</v>
       </c>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18" t="s">
+      <c r="H16" s="21"/>
+      <c r="I16" s="21" t="s">
         <v>235</v>
       </c>
-      <c r="J16" s="18"/>
-      <c r="K16" s="18" t="s">
+      <c r="J16" s="21"/>
+      <c r="K16" s="21" t="s">
         <v>236</v>
       </c>
-      <c r="L16" s="18"/>
-      <c r="M16" s="18" t="s">
+      <c r="L16" s="21"/>
+      <c r="M16" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="N16" s="18"/>
+      <c r="N16" s="21"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C17" s="4">
@@ -1980,26 +1972,26 @@
       <c r="B19" t="s">
         <v>152</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18" t="s">
+      <c r="D19" s="21"/>
+      <c r="E19" s="21" t="s">
         <v>233</v>
       </c>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18" t="s">
+      <c r="F19" s="21"/>
+      <c r="G19" s="21" t="s">
         <v>234</v>
       </c>
-      <c r="H19" s="18"/>
-      <c r="I19" s="19" t="s">
+      <c r="H19" s="21"/>
+      <c r="I19" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="20"/>
-      <c r="M19" s="20"/>
-      <c r="N19" s="21"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="23"/>
+      <c r="L19" s="23"/>
+      <c r="M19" s="23"/>
+      <c r="N19" s="24"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C20" s="4">
@@ -2033,18 +2025,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:N11"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="I8:N8"/>
     <mergeCell ref="M16:N16"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="E19:F19"/>
@@ -2055,17 +2035,29 @@
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="I16:J16"/>
     <mergeCell ref="K16:L16"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:N11"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="I8:N8"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:Z37"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView topLeftCell="B13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2077,28 +2069,28 @@
     <col min="7" max="7" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.28515625" style="1" customWidth="1"/>
     <col min="9" max="9" width="29" style="9" customWidth="1"/>
-    <col min="10" max="10" width="9.85546875" style="26" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" style="19" customWidth="1"/>
     <col min="12" max="12" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="L2" s="22" t="s">
+      <c r="L2" s="25" t="s">
         <v>281</v>
       </c>
-      <c r="M2" s="22"/>
-      <c r="N2" s="22"/>
-      <c r="O2" s="22"/>
-      <c r="P2" s="22"/>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="22"/>
-      <c r="S2" s="22"/>
-      <c r="T2" s="22"/>
-      <c r="U2" s="22"/>
-      <c r="V2" s="22"/>
-      <c r="W2" s="22"/>
-      <c r="X2" s="22"/>
-      <c r="Y2" s="22"/>
-      <c r="Z2" s="22"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="25"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="25"/>
+      <c r="Q2" s="25"/>
+      <c r="R2" s="25"/>
+      <c r="S2" s="25"/>
+      <c r="T2" s="25"/>
+      <c r="U2" s="25"/>
+      <c r="V2" s="25"/>
+      <c r="W2" s="25"/>
+      <c r="X2" s="25"/>
+      <c r="Y2" s="25"/>
+      <c r="Z2" s="25"/>
     </row>
     <row r="3" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -2125,13 +2117,13 @@
       <c r="I3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="27" t="s">
+      <c r="J3" s="20" t="s">
         <v>303</v>
       </c>
-      <c r="K3" s="14" t="s">
+      <c r="K3" s="13" t="s">
         <v>276</v>
       </c>
-      <c r="L3" s="15" t="s">
+      <c r="L3" s="14" t="s">
         <v>282</v>
       </c>
       <c r="M3" s="1" t="s">
@@ -2159,312 +2151,312 @@
         <v>290</v>
       </c>
     </row>
-    <row r="4" spans="2:26" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="16">
+    <row r="4" spans="2:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="15">
         <v>1</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="E4" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="F4" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="G4" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="17" t="s">
+      <c r="H4" s="16" t="s">
         <v>295</v>
       </c>
-      <c r="I4" s="17" t="s">
+      <c r="I4" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="J4" s="26" t="s">
+      <c r="J4" s="19" t="s">
         <v>301</v>
       </c>
-      <c r="K4" s="17" t="s">
+      <c r="K4" s="16" t="s">
         <v>277</v>
       </c>
-      <c r="L4" s="17" t="s">
+      <c r="L4" s="16" t="s">
         <v>291</v>
       </c>
-      <c r="M4" s="17" t="s">
+      <c r="M4" s="16" t="s">
         <v>292</v>
       </c>
-      <c r="N4" s="17" t="s">
+      <c r="N4" s="16" t="s">
         <v>291</v>
       </c>
-      <c r="O4" s="17" t="s">
+      <c r="O4" s="16" t="s">
         <v>291</v>
       </c>
-      <c r="P4" s="17" t="s">
+      <c r="P4" s="16" t="s">
         <v>291</v>
       </c>
-      <c r="Q4" s="17" t="s">
+      <c r="Q4" s="16" t="s">
         <v>291</v>
       </c>
-      <c r="R4" s="17" t="s">
+      <c r="R4" s="16" t="s">
         <v>293</v>
       </c>
-      <c r="S4" s="17" t="s">
+      <c r="S4" s="16" t="s">
         <v>291</v>
       </c>
-      <c r="T4" s="17"/>
-    </row>
-    <row r="5" spans="2:26" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="16">
+      <c r="T4" s="16"/>
+    </row>
+    <row r="5" spans="2:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="15">
         <f>B4+1</f>
         <v>2</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="17" t="s">
+      <c r="G5" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="17" t="s">
+      <c r="H5" s="16" t="s">
         <v>296</v>
       </c>
-      <c r="I5" s="17" t="s">
+      <c r="I5" s="16" t="s">
         <v>240</v>
       </c>
-      <c r="J5" s="26" t="s">
+      <c r="J5" s="19" t="s">
         <v>302</v>
       </c>
-      <c r="K5" s="17" t="s">
+      <c r="K5" s="16" t="s">
         <v>277</v>
       </c>
-      <c r="L5" s="17"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="17"/>
-      <c r="P5" s="17"/>
-      <c r="Q5" s="17"/>
-      <c r="R5" s="17"/>
-      <c r="S5" s="17"/>
-      <c r="T5" s="17"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="16"/>
+      <c r="R5" s="16"/>
+      <c r="S5" s="16"/>
+      <c r="T5" s="16"/>
     </row>
     <row r="6" spans="2:26" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="12">
         <f t="shared" ref="B6:B29" si="0">B5+1</f>
         <v>3</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="25" t="s">
+      <c r="E6" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="25" t="s">
+      <c r="F6" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="25" t="s">
+      <c r="G6" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="25" t="s">
+      <c r="H6" s="18" t="s">
         <v>297</v>
       </c>
-      <c r="I6" s="25" t="s">
+      <c r="I6" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="J6" s="26" t="s">
+      <c r="J6" s="19" t="s">
         <v>302</v>
       </c>
-      <c r="K6" s="25" t="s">
+      <c r="K6" s="18" t="s">
         <v>277</v>
       </c>
-      <c r="L6" s="25"/>
-      <c r="M6" s="25"/>
-      <c r="N6" s="25"/>
-      <c r="O6" s="25"/>
-      <c r="P6" s="25"/>
-      <c r="Q6" s="25"/>
-      <c r="R6" s="25"/>
-      <c r="S6" s="25"/>
-      <c r="T6" s="25"/>
-    </row>
-    <row r="7" spans="2:26" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="16">
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="18"/>
+      <c r="P6" s="18"/>
+      <c r="Q6" s="18"/>
+      <c r="R6" s="18"/>
+      <c r="S6" s="18"/>
+      <c r="T6" s="18"/>
+    </row>
+    <row r="7" spans="2:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="15">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E7" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17" t="s">
+      <c r="G7" s="16"/>
+      <c r="H7" s="16" t="s">
         <v>295</v>
       </c>
-      <c r="I7" s="17" t="s">
+      <c r="I7" s="16" t="s">
         <v>253</v>
       </c>
-      <c r="J7" s="26" t="s">
+      <c r="J7" s="19" t="s">
         <v>301</v>
       </c>
-      <c r="K7" s="17" t="s">
+      <c r="K7" s="16" t="s">
         <v>278</v>
       </c>
-      <c r="L7" s="17"/>
-      <c r="M7" s="17"/>
-      <c r="N7" s="17"/>
-      <c r="O7" s="17"/>
-      <c r="P7" s="17"/>
-      <c r="Q7" s="17"/>
-      <c r="R7" s="17"/>
-      <c r="S7" s="17"/>
-      <c r="T7" s="17"/>
-    </row>
-    <row r="8" spans="2:26" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="16">
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="16"/>
+      <c r="P7" s="16"/>
+      <c r="Q7" s="16"/>
+      <c r="R7" s="16"/>
+      <c r="S7" s="16"/>
+      <c r="T7" s="16"/>
+    </row>
+    <row r="8" spans="2:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="15">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="E8" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="F8" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="17" t="s">
+      <c r="G8" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="H8" s="17" t="s">
+      <c r="H8" s="16" t="s">
         <v>298</v>
       </c>
-      <c r="I8" s="17" t="s">
+      <c r="I8" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="J8" s="17" t="s">
+      <c r="J8" s="16" t="s">
         <v>305</v>
       </c>
-      <c r="K8" s="17" t="s">
+      <c r="K8" s="16" t="s">
         <v>278</v>
       </c>
-      <c r="L8" s="17"/>
-      <c r="M8" s="17"/>
-      <c r="N8" s="17"/>
-      <c r="O8" s="17"/>
-      <c r="P8" s="17"/>
-      <c r="Q8" s="17"/>
-      <c r="R8" s="17"/>
-      <c r="S8" s="17"/>
-      <c r="T8" s="17"/>
-    </row>
-    <row r="9" spans="2:26" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B9" s="16">
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="16"/>
+      <c r="P8" s="16"/>
+      <c r="Q8" s="16"/>
+      <c r="R8" s="16"/>
+      <c r="S8" s="16"/>
+      <c r="T8" s="16"/>
+    </row>
+    <row r="9" spans="2:26" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B9" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="17" t="s">
+      <c r="E9" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="24" t="s">
+      <c r="F9" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="G9" s="17" t="s">
+      <c r="G9" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="H9" s="17" t="s">
+      <c r="H9" s="16" t="s">
         <v>299</v>
       </c>
-      <c r="I9" s="17" t="s">
+      <c r="I9" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="J9" s="26" t="s">
+      <c r="J9" s="19" t="s">
         <v>304</v>
       </c>
-      <c r="K9" s="17" t="s">
+      <c r="K9" s="16" t="s">
         <v>279</v>
       </c>
-      <c r="L9" s="17"/>
-      <c r="M9" s="17"/>
-      <c r="N9" s="17"/>
-      <c r="O9" s="17"/>
-      <c r="P9" s="17"/>
-      <c r="Q9" s="17"/>
-      <c r="R9" s="17"/>
-      <c r="S9" s="17"/>
-      <c r="T9" s="17"/>
-    </row>
-    <row r="10" spans="2:26" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B10" s="16">
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="16"/>
+      <c r="Q9" s="16"/>
+      <c r="R9" s="16"/>
+      <c r="S9" s="16"/>
+      <c r="T9" s="16"/>
+    </row>
+    <row r="10" spans="2:26" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B10" s="15">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="E10" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="24" t="s">
+      <c r="F10" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="G10" s="17" t="s">
+      <c r="G10" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="H10" s="17" t="s">
+      <c r="H10" s="16" t="s">
         <v>300</v>
       </c>
-      <c r="I10" s="17" t="s">
+      <c r="I10" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="J10" s="26" t="s">
+      <c r="J10" s="19" t="s">
         <v>304</v>
       </c>
-      <c r="K10" s="17" t="s">
+      <c r="K10" s="16" t="s">
         <v>279</v>
       </c>
-      <c r="L10" s="17"/>
-      <c r="M10" s="17"/>
-      <c r="N10" s="17"/>
-      <c r="O10" s="17"/>
-      <c r="P10" s="17"/>
-      <c r="Q10" s="17"/>
-      <c r="R10" s="17"/>
-      <c r="S10" s="17"/>
-      <c r="T10" s="17"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="16"/>
+      <c r="P10" s="16"/>
+      <c r="Q10" s="16"/>
+      <c r="R10" s="16"/>
+      <c r="S10" s="16"/>
+      <c r="T10" s="16"/>
     </row>
     <row r="11" spans="2:26" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="10">
@@ -2490,7 +2482,7 @@
       <c r="I11" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="J11" s="26"/>
+      <c r="J11" s="19"/>
       <c r="K11" s="9"/>
       <c r="L11" s="9"/>
       <c r="M11" s="9"/>
@@ -2526,7 +2518,7 @@
       <c r="I12" s="9" t="s">
         <v>265</v>
       </c>
-      <c r="J12" s="26"/>
+      <c r="J12" s="19"/>
       <c r="K12" s="9"/>
       <c r="L12" s="9"/>
       <c r="M12" s="9"/>
@@ -2560,7 +2552,7 @@
       <c r="I13" s="9" t="s">
         <v>254</v>
       </c>
-      <c r="J13" s="26"/>
+      <c r="J13" s="19"/>
       <c r="K13" s="9" t="s">
         <v>277</v>
       </c>
@@ -2574,611 +2566,611 @@
       <c r="S13" s="9"/>
       <c r="T13" s="9"/>
     </row>
-    <row r="14" spans="2:26" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B14" s="16">
+    <row r="14" spans="2:26" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B14" s="15">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="D14" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="E14" s="17" t="s">
+      <c r="E14" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="24" t="s">
+      <c r="F14" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="G14" s="17" t="s">
+      <c r="G14" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17" t="s">
+      <c r="H14" s="16"/>
+      <c r="I14" s="16" t="s">
         <v>237</v>
       </c>
-      <c r="J14" s="26" t="s">
+      <c r="J14" s="19" t="s">
         <v>302</v>
       </c>
-      <c r="K14" s="17" t="s">
+      <c r="K14" s="16" t="s">
         <v>277</v>
       </c>
-      <c r="L14" s="17"/>
-      <c r="M14" s="17"/>
-      <c r="N14" s="17"/>
-      <c r="O14" s="17"/>
-      <c r="P14" s="17"/>
-      <c r="Q14" s="17"/>
-      <c r="R14" s="17"/>
-      <c r="S14" s="17"/>
-      <c r="T14" s="17"/>
-    </row>
-    <row r="15" spans="2:26" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="16">
+      <c r="L14" s="16"/>
+      <c r="M14" s="16"/>
+      <c r="N14" s="16"/>
+      <c r="O14" s="16"/>
+      <c r="P14" s="16"/>
+      <c r="Q14" s="16"/>
+      <c r="R14" s="16"/>
+      <c r="S14" s="16"/>
+      <c r="T14" s="16"/>
+    </row>
+    <row r="15" spans="2:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="15">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="D15" s="17" t="s">
+      <c r="D15" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="E15" s="17" t="s">
+      <c r="E15" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="F15" s="17" t="s">
+      <c r="F15" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="17" t="s">
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="J15" s="26" t="s">
+      <c r="J15" s="19" t="s">
         <v>279</v>
       </c>
-      <c r="K15" s="17"/>
-      <c r="L15" s="17"/>
-      <c r="M15" s="17"/>
-      <c r="N15" s="17"/>
-      <c r="O15" s="17"/>
-      <c r="P15" s="17"/>
-      <c r="Q15" s="17"/>
-      <c r="R15" s="17"/>
-      <c r="S15" s="17"/>
-      <c r="T15" s="17"/>
-    </row>
-    <row r="16" spans="2:26" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="16">
+      <c r="K15" s="16"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="16"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="16"/>
+      <c r="P15" s="16"/>
+      <c r="Q15" s="16"/>
+      <c r="R15" s="16"/>
+      <c r="S15" s="16"/>
+      <c r="T15" s="16"/>
+    </row>
+    <row r="16" spans="2:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="15">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C16" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="D16" s="17" t="s">
+      <c r="D16" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="E16" s="17" t="s">
+      <c r="E16" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="F16" s="17" t="s">
+      <c r="F16" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="G16" s="17" t="s">
+      <c r="G16" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17" t="s">
+      <c r="H16" s="16"/>
+      <c r="I16" s="16" t="s">
         <v>238</v>
       </c>
-      <c r="J16" s="26" t="s">
+      <c r="J16" s="19" t="s">
         <v>302</v>
       </c>
-      <c r="K16" s="17" t="s">
+      <c r="K16" s="16" t="s">
         <v>277</v>
       </c>
-      <c r="L16" s="17"/>
-      <c r="M16" s="17"/>
-      <c r="N16" s="17"/>
-      <c r="O16" s="17"/>
-      <c r="P16" s="17"/>
-      <c r="Q16" s="17"/>
-      <c r="R16" s="17"/>
-      <c r="S16" s="17"/>
-      <c r="T16" s="17"/>
-    </row>
-    <row r="17" spans="2:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="16">
+      <c r="L16" s="16"/>
+      <c r="M16" s="16"/>
+      <c r="N16" s="16"/>
+      <c r="O16" s="16"/>
+      <c r="P16" s="16"/>
+      <c r="Q16" s="16"/>
+      <c r="R16" s="16"/>
+      <c r="S16" s="16"/>
+      <c r="T16" s="16"/>
+    </row>
+    <row r="17" spans="2:20" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="15">
         <f>B16+1</f>
         <v>14</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="16" t="s">
         <v>245</v>
       </c>
-      <c r="D17" s="17" t="s">
+      <c r="D17" s="16" t="s">
         <v>246</v>
       </c>
-      <c r="E17" s="17" t="s">
+      <c r="E17" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="17" t="s">
+      <c r="F17" s="16" t="s">
         <v>247</v>
       </c>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17" t="s">
+      <c r="G17" s="16"/>
+      <c r="H17" s="16" t="s">
         <v>295</v>
       </c>
-      <c r="I17" s="17" t="s">
+      <c r="I17" s="16" t="s">
         <v>255</v>
       </c>
-      <c r="J17" s="26" t="s">
+      <c r="J17" s="19" t="s">
         <v>301</v>
       </c>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="17"/>
-      <c r="N17" s="17"/>
-      <c r="O17" s="17"/>
-      <c r="P17" s="17"/>
-      <c r="Q17" s="17"/>
-      <c r="R17" s="17"/>
-      <c r="S17" s="17"/>
-      <c r="T17" s="17"/>
-    </row>
-    <row r="18" spans="2:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="16">
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="16"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="16"/>
+      <c r="P17" s="16"/>
+      <c r="Q17" s="16"/>
+      <c r="R17" s="16"/>
+      <c r="S17" s="16"/>
+      <c r="T17" s="16"/>
+    </row>
+    <row r="18" spans="2:20" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="15">
         <f>B16+1</f>
         <v>14</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="D18" s="17" t="s">
+      <c r="D18" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="E18" s="17" t="s">
+      <c r="E18" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F18" s="17" t="s">
+      <c r="F18" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17" t="s">
+      <c r="G18" s="16"/>
+      <c r="H18" s="16" t="s">
         <v>295</v>
       </c>
-      <c r="I18" s="17" t="s">
+      <c r="I18" s="16" t="s">
         <v>256</v>
       </c>
-      <c r="J18" s="26" t="s">
+      <c r="J18" s="19" t="s">
         <v>301</v>
       </c>
-      <c r="K18" s="17"/>
-      <c r="L18" s="17"/>
-      <c r="M18" s="17"/>
-      <c r="N18" s="17"/>
-      <c r="O18" s="17"/>
-      <c r="P18" s="17"/>
-      <c r="Q18" s="17"/>
-      <c r="R18" s="17"/>
-      <c r="S18" s="17"/>
-      <c r="T18" s="17"/>
-    </row>
-    <row r="19" spans="2:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="16">
+      <c r="K18" s="16"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="16"/>
+      <c r="N18" s="16"/>
+      <c r="O18" s="16"/>
+      <c r="P18" s="16"/>
+      <c r="Q18" s="16"/>
+      <c r="R18" s="16"/>
+      <c r="S18" s="16"/>
+      <c r="T18" s="16"/>
+    </row>
+    <row r="19" spans="2:20" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="15">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C19" s="17" t="s">
+      <c r="C19" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="D19" s="17" t="s">
+      <c r="D19" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="E19" s="17" t="s">
+      <c r="E19" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F19" s="17" t="s">
+      <c r="F19" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17" t="s">
+      <c r="G19" s="16"/>
+      <c r="H19" s="16" t="s">
         <v>295</v>
       </c>
-      <c r="I19" s="17" t="s">
+      <c r="I19" s="16" t="s">
         <v>257</v>
       </c>
-      <c r="J19" s="26" t="s">
+      <c r="J19" s="19" t="s">
         <v>301</v>
       </c>
-      <c r="K19" s="17"/>
-      <c r="L19" s="17"/>
-      <c r="M19" s="17"/>
-      <c r="N19" s="17"/>
-      <c r="O19" s="17"/>
-      <c r="P19" s="17"/>
-      <c r="Q19" s="17"/>
-      <c r="R19" s="17"/>
-      <c r="S19" s="17"/>
-      <c r="T19" s="17"/>
-    </row>
-    <row r="20" spans="2:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="16">
+      <c r="K19" s="16"/>
+      <c r="L19" s="16"/>
+      <c r="M19" s="16"/>
+      <c r="N19" s="16"/>
+      <c r="O19" s="16"/>
+      <c r="P19" s="16"/>
+      <c r="Q19" s="16"/>
+      <c r="R19" s="16"/>
+      <c r="S19" s="16"/>
+      <c r="T19" s="16"/>
+    </row>
+    <row r="20" spans="2:20" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="15">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="C20" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="D20" s="17" t="s">
+      <c r="D20" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="E20" s="17" t="s">
+      <c r="E20" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="F20" s="17" t="s">
+      <c r="F20" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="G20" s="17" t="s">
+      <c r="G20" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="H20" s="17"/>
-      <c r="I20" s="17" t="s">
+      <c r="H20" s="16"/>
+      <c r="I20" s="16" t="s">
         <v>239</v>
       </c>
-      <c r="J20" s="17"/>
-      <c r="K20" s="17"/>
-      <c r="L20" s="17"/>
-      <c r="M20" s="17"/>
-      <c r="N20" s="17"/>
-      <c r="O20" s="17"/>
-      <c r="P20" s="17"/>
-      <c r="Q20" s="17"/>
-      <c r="R20" s="17"/>
-      <c r="S20" s="17"/>
-      <c r="T20" s="17"/>
-    </row>
-    <row r="21" spans="2:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="16">
+      <c r="J20" s="16"/>
+      <c r="K20" s="16"/>
+      <c r="L20" s="16"/>
+      <c r="M20" s="16"/>
+      <c r="N20" s="16"/>
+      <c r="O20" s="16"/>
+      <c r="P20" s="16"/>
+      <c r="Q20" s="16"/>
+      <c r="R20" s="16"/>
+      <c r="S20" s="16"/>
+      <c r="T20" s="16"/>
+    </row>
+    <row r="21" spans="2:20" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="15">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="C21" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="D21" s="17" t="s">
+      <c r="D21" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="E21" s="17" t="s">
+      <c r="E21" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F21" s="17" t="s">
+      <c r="F21" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17" t="s">
+      <c r="G21" s="16"/>
+      <c r="H21" s="16" t="s">
         <v>295</v>
       </c>
-      <c r="I21" s="17" t="s">
+      <c r="I21" s="16" t="s">
         <v>258</v>
       </c>
-      <c r="J21" s="26" t="s">
+      <c r="J21" s="19" t="s">
         <v>301</v>
       </c>
-      <c r="K21" s="17"/>
-      <c r="L21" s="17"/>
-      <c r="M21" s="17"/>
-      <c r="N21" s="17"/>
-      <c r="O21" s="17"/>
-      <c r="P21" s="17"/>
-      <c r="Q21" s="17"/>
-      <c r="R21" s="17"/>
-      <c r="S21" s="17"/>
-      <c r="T21" s="17"/>
-    </row>
-    <row r="22" spans="2:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="16">
+      <c r="K21" s="16"/>
+      <c r="L21" s="16"/>
+      <c r="M21" s="16"/>
+      <c r="N21" s="16"/>
+      <c r="O21" s="16"/>
+      <c r="P21" s="16"/>
+      <c r="Q21" s="16"/>
+      <c r="R21" s="16"/>
+      <c r="S21" s="16"/>
+      <c r="T21" s="16"/>
+    </row>
+    <row r="22" spans="2:20" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="15">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C22" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="D22" s="17" t="s">
+      <c r="D22" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="E22" s="17" t="s">
+      <c r="E22" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F22" s="17" t="s">
+      <c r="F22" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="G22" s="17" t="s">
+      <c r="G22" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="H22" s="17" t="s">
+      <c r="H22" s="16" t="s">
         <v>295</v>
       </c>
-      <c r="I22" s="17" t="s">
+      <c r="I22" s="16" t="s">
         <v>259</v>
       </c>
-      <c r="J22" s="26" t="s">
+      <c r="J22" s="19" t="s">
         <v>301</v>
       </c>
-      <c r="K22" s="17"/>
-      <c r="L22" s="17"/>
-      <c r="M22" s="17"/>
-      <c r="N22" s="17"/>
-      <c r="O22" s="17"/>
-      <c r="P22" s="17"/>
-      <c r="Q22" s="17"/>
-      <c r="R22" s="17"/>
-      <c r="S22" s="17"/>
-      <c r="T22" s="17"/>
-    </row>
-    <row r="23" spans="2:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="16">
+      <c r="K22" s="16"/>
+      <c r="L22" s="16"/>
+      <c r="M22" s="16"/>
+      <c r="N22" s="16"/>
+      <c r="O22" s="16"/>
+      <c r="P22" s="16"/>
+      <c r="Q22" s="16"/>
+      <c r="R22" s="16"/>
+      <c r="S22" s="16"/>
+      <c r="T22" s="16"/>
+    </row>
+    <row r="23" spans="2:20" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="15">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="C23" s="17" t="s">
+      <c r="C23" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="D23" s="17" t="s">
+      <c r="D23" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="E23" s="17" t="s">
+      <c r="E23" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F23" s="17" t="s">
+      <c r="F23" s="16" t="s">
         <v>274</v>
       </c>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17" t="s">
+      <c r="G23" s="16"/>
+      <c r="H23" s="16" t="s">
         <v>295</v>
       </c>
-      <c r="I23" s="17" t="s">
+      <c r="I23" s="16" t="s">
         <v>260</v>
       </c>
-      <c r="J23" s="26" t="s">
+      <c r="J23" s="19" t="s">
         <v>301</v>
       </c>
-      <c r="K23" s="17"/>
-      <c r="L23" s="17"/>
-      <c r="M23" s="17"/>
-      <c r="N23" s="17"/>
-      <c r="O23" s="17"/>
-      <c r="P23" s="17"/>
-      <c r="Q23" s="17"/>
-      <c r="R23" s="17"/>
-      <c r="S23" s="17"/>
-      <c r="T23" s="17"/>
-    </row>
-    <row r="24" spans="2:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="16">
+      <c r="K23" s="16"/>
+      <c r="L23" s="16"/>
+      <c r="M23" s="16"/>
+      <c r="N23" s="16"/>
+      <c r="O23" s="16"/>
+      <c r="P23" s="16"/>
+      <c r="Q23" s="16"/>
+      <c r="R23" s="16"/>
+      <c r="S23" s="16"/>
+      <c r="T23" s="16"/>
+    </row>
+    <row r="24" spans="2:20" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="15">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="C24" s="17" t="s">
+      <c r="C24" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="D24" s="17" t="s">
+      <c r="D24" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="E24" s="17" t="s">
+      <c r="E24" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F24" s="17" t="s">
+      <c r="F24" s="16" t="s">
         <v>275</v>
       </c>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17" t="s">
+      <c r="G24" s="16"/>
+      <c r="H24" s="16" t="s">
         <v>295</v>
       </c>
-      <c r="I24" s="17" t="s">
+      <c r="I24" s="16" t="s">
         <v>261</v>
       </c>
-      <c r="J24" s="26" t="s">
+      <c r="J24" s="19" t="s">
         <v>301</v>
       </c>
-      <c r="K24" s="17"/>
-      <c r="L24" s="17"/>
-      <c r="M24" s="17"/>
-      <c r="N24" s="17"/>
-      <c r="O24" s="17"/>
-      <c r="P24" s="17"/>
-      <c r="Q24" s="17"/>
-      <c r="R24" s="17"/>
-      <c r="S24" s="17"/>
-      <c r="T24" s="17"/>
-    </row>
-    <row r="25" spans="2:20" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B25" s="16">
+      <c r="K24" s="16"/>
+      <c r="L24" s="16"/>
+      <c r="M24" s="16"/>
+      <c r="N24" s="16"/>
+      <c r="O24" s="16"/>
+      <c r="P24" s="16"/>
+      <c r="Q24" s="16"/>
+      <c r="R24" s="16"/>
+      <c r="S24" s="16"/>
+      <c r="T24" s="16"/>
+    </row>
+    <row r="25" spans="2:20" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B25" s="15">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="C25" s="17" t="s">
+      <c r="C25" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="D25" s="17" t="s">
+      <c r="D25" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="E25" s="17" t="s">
+      <c r="E25" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="F25" s="24" t="s">
+      <c r="F25" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="G25" s="17" t="s">
+      <c r="G25" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="H25" s="17"/>
-      <c r="I25" s="17" t="s">
+      <c r="H25" s="16"/>
+      <c r="I25" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="J25" s="26" t="s">
+      <c r="J25" s="19" t="s">
         <v>302</v>
       </c>
-      <c r="K25" s="17"/>
-      <c r="L25" s="17"/>
-      <c r="M25" s="17"/>
-      <c r="N25" s="17"/>
-      <c r="O25" s="17"/>
-      <c r="P25" s="17"/>
-      <c r="Q25" s="17"/>
-      <c r="R25" s="17"/>
-      <c r="S25" s="17"/>
-      <c r="T25" s="17"/>
-    </row>
-    <row r="26" spans="2:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="16">
+      <c r="K25" s="16"/>
+      <c r="L25" s="16"/>
+      <c r="M25" s="16"/>
+      <c r="N25" s="16"/>
+      <c r="O25" s="16"/>
+      <c r="P25" s="16"/>
+      <c r="Q25" s="16"/>
+      <c r="R25" s="16"/>
+      <c r="S25" s="16"/>
+      <c r="T25" s="16"/>
+    </row>
+    <row r="26" spans="2:20" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="15">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="C26" s="17" t="s">
+      <c r="C26" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="D26" s="17" t="s">
+      <c r="D26" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="E26" s="17" t="s">
+      <c r="E26" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="F26" s="17" t="s">
+      <c r="F26" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="G26" s="17" t="s">
+      <c r="G26" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="H26" s="17"/>
-      <c r="I26" s="17" t="s">
+      <c r="H26" s="16"/>
+      <c r="I26" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="J26" s="26" t="s">
+      <c r="J26" s="19" t="s">
         <v>302</v>
       </c>
-      <c r="K26" s="17"/>
-      <c r="L26" s="17"/>
-      <c r="M26" s="17"/>
-      <c r="N26" s="17"/>
-      <c r="O26" s="17"/>
-      <c r="P26" s="17"/>
-      <c r="Q26" s="17"/>
-      <c r="R26" s="17"/>
-      <c r="S26" s="17"/>
-      <c r="T26" s="17"/>
-    </row>
-    <row r="27" spans="2:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="16">
+      <c r="K26" s="16"/>
+      <c r="L26" s="16"/>
+      <c r="M26" s="16"/>
+      <c r="N26" s="16"/>
+      <c r="O26" s="16"/>
+      <c r="P26" s="16"/>
+      <c r="Q26" s="16"/>
+      <c r="R26" s="16"/>
+      <c r="S26" s="16"/>
+      <c r="T26" s="16"/>
+    </row>
+    <row r="27" spans="2:20" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="15">
         <f>B26+1</f>
         <v>23</v>
       </c>
-      <c r="C27" s="17" t="s">
+      <c r="C27" s="16" t="s">
         <v>242</v>
       </c>
-      <c r="D27" s="17" t="s">
+      <c r="D27" s="16" t="s">
         <v>243</v>
       </c>
-      <c r="E27" s="17" t="s">
+      <c r="E27" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F27" s="17" t="s">
+      <c r="F27" s="16" t="s">
         <v>244</v>
       </c>
-      <c r="G27" s="17"/>
-      <c r="H27" s="17"/>
-      <c r="I27" s="17" t="s">
+      <c r="G27" s="16"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="16" t="s">
         <v>262</v>
       </c>
-      <c r="J27" s="26" t="s">
+      <c r="J27" s="19" t="s">
         <v>301</v>
       </c>
-      <c r="K27" s="17"/>
-      <c r="L27" s="17"/>
-      <c r="M27" s="17"/>
-      <c r="N27" s="17"/>
-      <c r="O27" s="17"/>
-      <c r="P27" s="17"/>
-      <c r="Q27" s="17"/>
-      <c r="R27" s="17"/>
-      <c r="S27" s="17"/>
-      <c r="T27" s="17"/>
-    </row>
-    <row r="28" spans="2:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="16">
+      <c r="K27" s="16"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="16"/>
+      <c r="N27" s="16"/>
+      <c r="O27" s="16"/>
+      <c r="P27" s="16"/>
+      <c r="Q27" s="16"/>
+      <c r="R27" s="16"/>
+      <c r="S27" s="16"/>
+      <c r="T27" s="16"/>
+    </row>
+    <row r="28" spans="2:20" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="15">
         <f>B26+1</f>
         <v>23</v>
       </c>
-      <c r="C28" s="17" t="s">
+      <c r="C28" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="D28" s="17" t="s">
+      <c r="D28" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="E28" s="17" t="s">
+      <c r="E28" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F28" s="17" t="s">
+      <c r="F28" s="16" t="s">
         <v>241</v>
       </c>
-      <c r="G28" s="17" t="s">
+      <c r="G28" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="H28" s="17"/>
-      <c r="I28" s="17" t="s">
+      <c r="H28" s="16"/>
+      <c r="I28" s="16" t="s">
         <v>263</v>
       </c>
-      <c r="J28" s="26" t="s">
+      <c r="J28" s="19" t="s">
         <v>301</v>
       </c>
-      <c r="K28" s="17"/>
-      <c r="L28" s="17"/>
-      <c r="M28" s="17"/>
-      <c r="N28" s="17"/>
-      <c r="O28" s="17"/>
-      <c r="P28" s="17"/>
-      <c r="Q28" s="17"/>
-      <c r="R28" s="17"/>
-      <c r="S28" s="17"/>
-      <c r="T28" s="17"/>
-    </row>
-    <row r="29" spans="2:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="16">
+      <c r="K28" s="16"/>
+      <c r="L28" s="16"/>
+      <c r="M28" s="16"/>
+      <c r="N28" s="16"/>
+      <c r="O28" s="16"/>
+      <c r="P28" s="16"/>
+      <c r="Q28" s="16"/>
+      <c r="R28" s="16"/>
+      <c r="S28" s="16"/>
+      <c r="T28" s="16"/>
+    </row>
+    <row r="29" spans="2:20" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="15">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="C29" s="17" t="s">
+      <c r="C29" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="D29" s="17" t="s">
+      <c r="D29" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="E29" s="17" t="s">
+      <c r="E29" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F29" s="17" t="s">
+      <c r="F29" s="16" t="s">
         <v>241</v>
       </c>
-      <c r="G29" s="17"/>
-      <c r="H29" s="17"/>
-      <c r="I29" s="17" t="s">
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="16" t="s">
         <v>264</v>
       </c>
-      <c r="J29" s="26" t="s">
+      <c r="J29" s="19" t="s">
         <v>301</v>
       </c>
-      <c r="K29" s="17"/>
-      <c r="L29" s="17"/>
-      <c r="M29" s="17"/>
-      <c r="N29" s="17"/>
-      <c r="O29" s="17"/>
-      <c r="P29" s="17"/>
-      <c r="Q29" s="17"/>
-      <c r="R29" s="17"/>
-      <c r="S29" s="17"/>
-      <c r="T29" s="17"/>
+      <c r="K29" s="16"/>
+      <c r="L29" s="16"/>
+      <c r="M29" s="16"/>
+      <c r="N29" s="16"/>
+      <c r="O29" s="16"/>
+      <c r="P29" s="16"/>
+      <c r="Q29" s="16"/>
+      <c r="R29" s="16"/>
+      <c r="S29" s="16"/>
+      <c r="T29" s="16"/>
     </row>
     <row r="31" spans="2:20" x14ac:dyDescent="0.25">
       <c r="F31" s="1" t="s">
@@ -3228,7 +3220,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3445,11 +3437,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3531,20 +3523,20 @@
     </row>
     <row r="6" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="16" t="s">
         <v>159</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="16" t="s">
         <v>160</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="16" t="s">
         <v>161</v>
       </c>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17" t="s">
+      <c r="F6" s="16"/>
+      <c r="G6" s="16" t="s">
         <v>266</v>
       </c>
       <c r="H6" s="9" t="s">
@@ -3552,22 +3544,22 @@
       </c>
     </row>
     <row r="7" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="16" t="s">
         <v>162</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="16" t="s">
         <v>163</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E7" s="16" t="s">
         <v>161</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="G7" s="17" t="s">
+      <c r="G7" s="16" t="s">
         <v>267</v>
       </c>
       <c r="H7" s="9" t="s">
@@ -3630,13 +3622,13 @@
       <c r="G10" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="H10" s="23" t="s">
+      <c r="H10" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="I10" s="23"/>
-      <c r="J10" s="23"/>
-      <c r="K10" s="23"/>
-      <c r="L10" s="23"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="26"/>
+      <c r="K10" s="26"/>
+      <c r="L10" s="26"/>
     </row>
     <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
@@ -3655,11 +3647,11 @@
       <c r="G11" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="H11" s="23"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="23"/>
-      <c r="K11" s="23"/>
-      <c r="L11" s="23"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="26"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
@@ -3746,7 +3738,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>197</v>
       </c>
@@ -3763,7 +3755,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12"/>
       <c r="B18" s="9" t="s">
         <v>200</v>
@@ -3784,7 +3776,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
       <c r="B19" s="9" t="s">
         <v>204</v>
@@ -3805,122 +3797,135 @@
         <v>148</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="12"/>
-      <c r="B20" s="9" t="s">
+    <row r="20" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="16" t="s">
         <v>207</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="16" t="s">
         <v>208</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D20" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="E20" s="16" t="s">
         <v>209</v>
       </c>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9" t="s">
+      <c r="F20" s="16"/>
+      <c r="G20" s="16" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="12"/>
-      <c r="B21" s="9" t="s">
+      <c r="H20" s="16" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="16" t="s">
         <v>210</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="16" t="s">
         <v>211</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D21" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="E21" s="16" t="s">
         <v>212</v>
       </c>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9" t="s">
+      <c r="F21" s="16"/>
+      <c r="G21" s="16" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="12"/>
-      <c r="B22" s="9" t="s">
+      <c r="H21" s="16" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="16" t="s">
         <v>213</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="16" t="s">
         <v>214</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="D22" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="E22" s="13" t="s">
+      <c r="E22" s="16" t="s">
         <v>215</v>
       </c>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9" t="s">
+      <c r="F22" s="16"/>
+      <c r="G22" s="16" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
-      <c r="B23" s="9" t="s">
+      <c r="H22" s="16" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="16" t="s">
         <v>217</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="16" t="s">
         <v>218</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="D23" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="E23" s="9" t="s">
+      <c r="E23" s="16" t="s">
         <v>219</v>
       </c>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9" t="s">
+      <c r="F23" s="16"/>
+      <c r="G23" s="16" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="9" t="s">
+      <c r="H23" s="16" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="16" t="s">
         <v>220</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C24" s="16" t="s">
         <v>221</v>
       </c>
-      <c r="D24" s="9" t="s">
+      <c r="D24" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="E24" s="9" t="s">
+      <c r="E24" s="16" t="s">
         <v>222</v>
       </c>
-      <c r="F24" s="9" t="s">
+      <c r="F24" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="G24" s="9" t="s">
+      <c r="G24" s="16" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="12"/>
-      <c r="B25" s="9" t="s">
+      <c r="H24" s="16" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="16" t="s">
         <v>223</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C25" s="16" t="s">
         <v>224</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="D25" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="E25" s="9" t="s">
+      <c r="E25" s="16" t="s">
         <v>225</v>
       </c>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9" t="s">
+      <c r="F25" s="16"/>
+      <c r="G25" s="16" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H25" s="16" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="12"/>
       <c r="B26" s="9" t="s">
         <v>226</v>
@@ -3941,7 +3946,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="12"/>
       <c r="B27" s="1" t="s">
         <v>230</v>

</xml_diff>

<commit_message>
Adjusted Float Registers for multiple writes/reads, and implemented more functions in ALU/ALU control
</commit_message>
<xml_diff>
--- a/IS.xlsx
+++ b/IS.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a.akasheh\Documents\Quartus\modifiedMIPS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Okasha\Documents\modifiedMIPS\modifiedMIPS\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6575C3DE-3734-4D62-9FBE-0CCCA10F19F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3405" windowWidth="11970" windowHeight="10200" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instr. Formats" sheetId="2" r:id="rId1"/>
@@ -17,7 +18,7 @@
     <sheet name="Registers" sheetId="3" r:id="rId3"/>
     <sheet name="Floating" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="311">
   <si>
     <t>FORMAT</t>
   </si>
@@ -963,12 +964,21 @@
   </si>
   <si>
     <t>101</t>
+  </si>
+  <si>
+    <t>011</t>
+  </si>
+  <si>
+    <t>110</t>
+  </si>
+  <si>
+    <t>111</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1401,57 +1411,57 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B3:T29" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="B3:T29" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
   <tableColumns count="19">
-    <tableColumn id="1" name="No." dataDxfId="31">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="No." dataDxfId="31">
       <calculatedColumnFormula>B3+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="NAME" dataDxfId="30"/>
-    <tableColumn id="3" name="MNEMONIC" dataDxfId="29"/>
-    <tableColumn id="4" name="FORMAT" dataDxfId="28"/>
-    <tableColumn id="5" name="OPERATION (in Verilog)" dataDxfId="27"/>
-    <tableColumn id="6" name="Note" dataDxfId="26"/>
-    <tableColumn id="18" name="OPCODE zay el kheleg" dataDxfId="25"/>
-    <tableColumn id="7" name="OPCODE/ FUNCT(Hex)" dataDxfId="24"/>
-    <tableColumn id="19" name="ALU Opc" dataDxfId="23"/>
-    <tableColumn id="8" name="ALU OP" dataDxfId="22"/>
-    <tableColumn id="9" name="MemWrite" dataDxfId="21"/>
-    <tableColumn id="10" name="RegWrite" dataDxfId="20"/>
-    <tableColumn id="11" name="ALUs" dataDxfId="19"/>
-    <tableColumn id="12" name="Float" dataDxfId="18"/>
-    <tableColumn id="13" name="RegDst" dataDxfId="17"/>
-    <tableColumn id="14" name="HiLoWrite" dataDxfId="16"/>
-    <tableColumn id="15" name="HL" dataDxfId="15"/>
-    <tableColumn id="16" name="WBSrc" dataDxfId="14"/>
-    <tableColumn id="17" name="ALUc" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="NAME" dataDxfId="30"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="MNEMONIC" dataDxfId="29"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="FORMAT" dataDxfId="28"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="OPERATION (in Verilog)" dataDxfId="27"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Note" dataDxfId="26"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="OPCODE zay el kheleg" dataDxfId="25"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="OPCODE/ FUNCT(Hex)" dataDxfId="24"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="ALU Opc" dataDxfId="23"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="ALU OP" dataDxfId="22"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="MemWrite" dataDxfId="21"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="RegWrite" dataDxfId="20"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="ALUs" dataDxfId="19"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Float" dataDxfId="18"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="RegDst" dataDxfId="17"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="HiLoWrite" dataDxfId="16"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="HL" dataDxfId="15"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="WBSrc" dataDxfId="14"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="ALUc" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B3:E14" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="B3:E14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="B3:E14" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="B3:E14" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="NAME" dataDxfId="10"/>
-    <tableColumn id="2" name="NUMBER" dataDxfId="9"/>
-    <tableColumn id="3" name="USE" dataDxfId="8"/>
-    <tableColumn id="4" name="PRESERVED ACROSS A CALL?" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="NAME" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="NUMBER" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="USE" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="PRESERVED ACROSS A CALL?" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B3:G27" totalsRowShown="0" headerRowDxfId="6">
-  <autoFilter ref="B3:G27"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table3" displayName="Table3" ref="B3:G27" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="B3:G27" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="NAME" dataDxfId="5"/>
-    <tableColumn id="2" name="MNEMONIC" dataDxfId="4"/>
-    <tableColumn id="3" name="FORMAT" dataDxfId="3"/>
-    <tableColumn id="4" name="OPERATION" dataDxfId="2"/>
-    <tableColumn id="5" name="Note" dataDxfId="1"/>
-    <tableColumn id="6" name="Opcode/ FMT /FT/ FUNCT(Hex)" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="NAME" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="MNEMONIC" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="FORMAT" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="OPERATION" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Note" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Opcode/ FMT /FT/ FUNCT(Hex)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1719,11 +1729,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:N20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K5" sqref="K5:L5"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2025,18 +2035,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:N11"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="I8:N8"/>
     <mergeCell ref="M16:N16"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="E19:F19"/>
@@ -2047,17 +2045,29 @@
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="I16:J16"/>
     <mergeCell ref="K16:L16"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:N11"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="I8:N8"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:Z37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2443,7 +2453,7 @@
         <v>33</v>
       </c>
       <c r="J10" s="18" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="K10" s="15" t="s">
         <v>279</v>
@@ -3222,10 +3232,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B3:E19"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -3439,11 +3449,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:L27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A3:N27"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3451,12 +3461,12 @@
     <col min="2" max="2" width="18.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="10" style="1" customWidth="1"/>
-    <col min="5" max="5" width="27.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.5703125" style="1" customWidth="1"/>
     <col min="6" max="6" width="8.85546875" style="1"/>
     <col min="7" max="7" width="31.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
@@ -3479,52 +3489,53 @@
         <v>306</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="1" t="s">
+    <row r="4" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="15" t="s">
         <v>152</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="15" t="s">
         <v>153</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="15" t="s">
         <v>154</v>
       </c>
-      <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="1" t="s">
+      <c r="H4" s="15" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="15" t="s">
         <v>155</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="15" t="s">
         <v>156</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="15" t="s">
         <v>152</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="15" t="s">
         <v>157</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="15" t="s">
         <v>158</v>
       </c>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
+      <c r="H5" s="15" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="15" t="s">
         <v>159</v>
       </c>
@@ -3541,11 +3552,11 @@
       <c r="G6" s="15" t="s">
         <v>266</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="15" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="15" t="s">
         <v>162</v>
       </c>
@@ -3564,11 +3575,11 @@
       <c r="G7" s="15" t="s">
         <v>267</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="15" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
       <c r="B8" s="9" t="s">
         <v>164</v>
@@ -3588,7 +3599,7 @@
       </c>
       <c r="H8" s="9"/>
     </row>
-    <row r="9" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
       <c r="B9" s="1" t="s">
         <v>169</v>
@@ -3607,7 +3618,7 @@
       </c>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
       <c r="B10" s="1" t="s">
         <v>172</v>
@@ -3631,8 +3642,11 @@
       <c r="J10" s="25"/>
       <c r="K10" s="25"/>
       <c r="L10" s="25"/>
-    </row>
-    <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="N10">
+        <v>110010</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
       <c r="B11" s="1" t="s">
         <v>176</v>
@@ -3654,8 +3668,11 @@
       <c r="J11" s="25"/>
       <c r="K11" s="25"/>
       <c r="L11" s="25"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N11">
+        <v>111100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>179</v>
       </c>
@@ -3671,8 +3688,11 @@
       <c r="G12" s="1" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="N12">
+        <v>111110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>183</v>
       </c>
@@ -3689,7 +3709,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>186</v>
       </c>
@@ -3706,7 +3726,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>190</v>
       </c>
@@ -3723,7 +3743,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>193</v>
       </c>

</xml_diff>

<commit_message>
modified the EX stage for additional instruction support
</commit_message>
<xml_diff>
--- a/IS.xlsx
+++ b/IS.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Okasha\Documents\modifiedMIPS\modifiedMIPS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a.akasheh\Documents\Quartus\modifiedMIPS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6575C3DE-3734-4D62-9FBE-0CCCA10F19F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Instr. Formats" sheetId="2" r:id="rId1"/>
@@ -18,7 +17,7 @@
     <sheet name="Registers" sheetId="3" r:id="rId3"/>
     <sheet name="Floating" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="310">
   <si>
     <t>FORMAT</t>
   </si>
@@ -967,9 +966,6 @@
   </si>
   <si>
     <t>011</t>
-  </si>
-  <si>
-    <t>110</t>
   </si>
   <si>
     <t>111</t>
@@ -978,7 +974,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1411,57 +1407,57 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="B3:T29" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B3:T29" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="No." dataDxfId="31">
+    <tableColumn id="1" name="No." dataDxfId="31">
       <calculatedColumnFormula>B3+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="NAME" dataDxfId="30"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="MNEMONIC" dataDxfId="29"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="FORMAT" dataDxfId="28"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="OPERATION (in Verilog)" dataDxfId="27"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Note" dataDxfId="26"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="OPCODE zay el kheleg" dataDxfId="25"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="OPCODE/ FUNCT(Hex)" dataDxfId="24"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="ALU Opc" dataDxfId="23"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="ALU OP" dataDxfId="22"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="MemWrite" dataDxfId="21"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="RegWrite" dataDxfId="20"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="ALUs" dataDxfId="19"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Float" dataDxfId="18"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="RegDst" dataDxfId="17"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="HiLoWrite" dataDxfId="16"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="HL" dataDxfId="15"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="WBSrc" dataDxfId="14"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="ALUc" dataDxfId="13"/>
+    <tableColumn id="2" name="NAME" dataDxfId="30"/>
+    <tableColumn id="3" name="MNEMONIC" dataDxfId="29"/>
+    <tableColumn id="4" name="FORMAT" dataDxfId="28"/>
+    <tableColumn id="5" name="OPERATION (in Verilog)" dataDxfId="27"/>
+    <tableColumn id="6" name="Note" dataDxfId="26"/>
+    <tableColumn id="18" name="OPCODE zay el kheleg" dataDxfId="25"/>
+    <tableColumn id="7" name="OPCODE/ FUNCT(Hex)" dataDxfId="24"/>
+    <tableColumn id="19" name="ALU Opc" dataDxfId="23"/>
+    <tableColumn id="8" name="ALU OP" dataDxfId="22"/>
+    <tableColumn id="9" name="MemWrite" dataDxfId="21"/>
+    <tableColumn id="10" name="RegWrite" dataDxfId="20"/>
+    <tableColumn id="11" name="ALUs" dataDxfId="19"/>
+    <tableColumn id="12" name="Float" dataDxfId="18"/>
+    <tableColumn id="13" name="RegDst" dataDxfId="17"/>
+    <tableColumn id="14" name="HiLoWrite" dataDxfId="16"/>
+    <tableColumn id="15" name="HL" dataDxfId="15"/>
+    <tableColumn id="16" name="WBSrc" dataDxfId="14"/>
+    <tableColumn id="17" name="ALUc" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="B3:E14" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="B3:E14" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B3:E14" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="B3:E14"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="NAME" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="NUMBER" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="USE" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="PRESERVED ACROSS A CALL?" dataDxfId="7"/>
+    <tableColumn id="1" name="NAME" dataDxfId="10"/>
+    <tableColumn id="2" name="NUMBER" dataDxfId="9"/>
+    <tableColumn id="3" name="USE" dataDxfId="8"/>
+    <tableColumn id="4" name="PRESERVED ACROSS A CALL?" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table3" displayName="Table3" ref="B3:G27" totalsRowShown="0" headerRowDxfId="6">
-  <autoFilter ref="B3:G27" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B3:G27" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="B3:G27"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="NAME" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="MNEMONIC" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="FORMAT" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="OPERATION" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Note" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Opcode/ FMT /FT/ FUNCT(Hex)" dataDxfId="0"/>
+    <tableColumn id="1" name="NAME" dataDxfId="5"/>
+    <tableColumn id="2" name="MNEMONIC" dataDxfId="4"/>
+    <tableColumn id="3" name="FORMAT" dataDxfId="3"/>
+    <tableColumn id="4" name="OPERATION" dataDxfId="2"/>
+    <tableColumn id="5" name="Note" dataDxfId="1"/>
+    <tableColumn id="6" name="Opcode/ FMT /FT/ FUNCT(Hex)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1729,7 +1725,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:N20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2035,6 +2031,18 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:N11"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="I8:N8"/>
     <mergeCell ref="M16:N16"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="E19:F19"/>
@@ -2045,29 +2053,17 @@
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="I16:J16"/>
     <mergeCell ref="K16:L16"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:N11"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="I8:N8"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:Z37"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3232,7 +3228,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3449,11 +3445,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:G11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3532,7 +3528,7 @@
         <v>158</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="6" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -3597,7 +3593,9 @@
       <c r="G8" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="H8" s="9"/>
+      <c r="H8" s="9" t="s">
+        <v>309</v>
+      </c>
     </row>
     <row r="9" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
@@ -3616,7 +3614,9 @@
       <c r="G9" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="H9" s="1"/>
+      <c r="H9" s="1" t="s">
+        <v>309</v>
+      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
@@ -3635,13 +3635,9 @@
       <c r="G10" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="H10" s="25" t="s">
-        <v>144</v>
-      </c>
-      <c r="I10" s="25"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="25"/>
-      <c r="L10" s="25"/>
+      <c r="H10" s="1" t="s">
+        <v>309</v>
+      </c>
       <c r="N10">
         <v>110010</v>
       </c>
@@ -3663,11 +3659,9 @@
       <c r="G11" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="H11" s="25"/>
-      <c r="I11" s="25"/>
-      <c r="J11" s="25"/>
-      <c r="K11" s="25"/>
-      <c r="L11" s="25"/>
+      <c r="H11" s="1" t="s">
+        <v>309</v>
+      </c>
       <c r="N11">
         <v>111100</v>
       </c>
@@ -3692,7 +3686,7 @@
         <v>111110</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>183</v>
       </c>
@@ -3708,6 +3702,13 @@
       <c r="G13" s="1" t="s">
         <v>145</v>
       </c>
+      <c r="I13" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="J13" s="25"/>
+      <c r="K13" s="25"/>
+      <c r="L13" s="25"/>
+      <c r="M13" s="25"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
@@ -3725,6 +3726,11 @@
       <c r="G14" s="1" t="s">
         <v>189</v>
       </c>
+      <c r="I14" s="25"/>
+      <c r="J14" s="25"/>
+      <c r="K14" s="25"/>
+      <c r="L14" s="25"/>
+      <c r="M14" s="25"/>
     </row>
     <row r="15" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
@@ -3800,7 +3806,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="19" spans="2:8" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B19" s="15" t="s">
         <v>204</v>
       </c>
@@ -3974,7 +3980,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="27" spans="2:8" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B27" s="15" t="s">
         <v>230</v>
       </c>
@@ -3999,7 +4005,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="H10:L11"/>
+    <mergeCell ref="I13:M14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added more instruction support to EX
</commit_message>
<xml_diff>
--- a/IS.xlsx
+++ b/IS.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a.akasheh\Documents\Quartus\modifiedMIPS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Okasha\Documents\modifiedMIPS\modifiedMIPS\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13DDFFFC-C0FD-4725-B7CD-3B28A2B59B0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="-5970" yWindow="4335" windowWidth="11970" windowHeight="10200" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instr. Formats" sheetId="2" r:id="rId1"/>
@@ -17,7 +18,7 @@
     <sheet name="Registers" sheetId="3" r:id="rId3"/>
     <sheet name="Floating" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -974,7 +975,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1407,57 +1408,57 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B3:T29" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="B3:T29" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
   <tableColumns count="19">
-    <tableColumn id="1" name="No." dataDxfId="31">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="No." dataDxfId="31">
       <calculatedColumnFormula>B3+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="NAME" dataDxfId="30"/>
-    <tableColumn id="3" name="MNEMONIC" dataDxfId="29"/>
-    <tableColumn id="4" name="FORMAT" dataDxfId="28"/>
-    <tableColumn id="5" name="OPERATION (in Verilog)" dataDxfId="27"/>
-    <tableColumn id="6" name="Note" dataDxfId="26"/>
-    <tableColumn id="18" name="OPCODE zay el kheleg" dataDxfId="25"/>
-    <tableColumn id="7" name="OPCODE/ FUNCT(Hex)" dataDxfId="24"/>
-    <tableColumn id="19" name="ALU Opc" dataDxfId="23"/>
-    <tableColumn id="8" name="ALU OP" dataDxfId="22"/>
-    <tableColumn id="9" name="MemWrite" dataDxfId="21"/>
-    <tableColumn id="10" name="RegWrite" dataDxfId="20"/>
-    <tableColumn id="11" name="ALUs" dataDxfId="19"/>
-    <tableColumn id="12" name="Float" dataDxfId="18"/>
-    <tableColumn id="13" name="RegDst" dataDxfId="17"/>
-    <tableColumn id="14" name="HiLoWrite" dataDxfId="16"/>
-    <tableColumn id="15" name="HL" dataDxfId="15"/>
-    <tableColumn id="16" name="WBSrc" dataDxfId="14"/>
-    <tableColumn id="17" name="ALUc" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="NAME" dataDxfId="30"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="MNEMONIC" dataDxfId="29"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="FORMAT" dataDxfId="28"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="OPERATION (in Verilog)" dataDxfId="27"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Note" dataDxfId="26"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="OPCODE zay el kheleg" dataDxfId="25"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="OPCODE/ FUNCT(Hex)" dataDxfId="24"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="ALU Opc" dataDxfId="23"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="ALU OP" dataDxfId="22"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="MemWrite" dataDxfId="21"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="RegWrite" dataDxfId="20"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="ALUs" dataDxfId="19"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Float" dataDxfId="18"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="RegDst" dataDxfId="17"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="HiLoWrite" dataDxfId="16"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="HL" dataDxfId="15"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="WBSrc" dataDxfId="14"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="ALUc" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B3:E14" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="B3:E14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="B3:E14" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="B3:E14" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="NAME" dataDxfId="10"/>
-    <tableColumn id="2" name="NUMBER" dataDxfId="9"/>
-    <tableColumn id="3" name="USE" dataDxfId="8"/>
-    <tableColumn id="4" name="PRESERVED ACROSS A CALL?" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="NAME" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="NUMBER" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="USE" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="PRESERVED ACROSS A CALL?" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B3:G27" totalsRowShown="0" headerRowDxfId="6">
-  <autoFilter ref="B3:G27"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table3" displayName="Table3" ref="B3:G27" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="B3:G27" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="NAME" dataDxfId="5"/>
-    <tableColumn id="2" name="MNEMONIC" dataDxfId="4"/>
-    <tableColumn id="3" name="FORMAT" dataDxfId="3"/>
-    <tableColumn id="4" name="OPERATION" dataDxfId="2"/>
-    <tableColumn id="5" name="Note" dataDxfId="1"/>
-    <tableColumn id="6" name="Opcode/ FMT /FT/ FUNCT(Hex)" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="NAME" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="MNEMONIC" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="FORMAT" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="OPERATION" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Note" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Opcode/ FMT /FT/ FUNCT(Hex)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1725,11 +1726,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:N20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="E16" sqref="E16:F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2031,18 +2032,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:N11"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="I8:N8"/>
     <mergeCell ref="M16:N16"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="E19:F19"/>
@@ -2053,16 +2042,28 @@
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="I16:J16"/>
     <mergeCell ref="K16:L16"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:N11"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="I8:N8"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:Z37"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
@@ -3228,7 +3229,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B3:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3445,11 +3446,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A3:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added Hazard and Forwarding Compatibility
</commit_message>
<xml_diff>
--- a/IS.xlsx
+++ b/IS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Okasha\Documents\modifiedMIPS\modifiedMIPS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B32C024-7915-4813-B751-50F5E35530BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB1DE106-FE76-424A-9CD1-97E91C3D377C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21660" yWindow="6345" windowWidth="13875" windowHeight="10200" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instr. Formats" sheetId="2" r:id="rId1"/>
@@ -1169,6 +1169,12 @@
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1187,12 +1193,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1775,30 +1775,30 @@
       <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18" t="s">
+      <c r="D5" s="24"/>
+      <c r="E5" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18" t="s">
+      <c r="F5" s="24"/>
+      <c r="G5" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18" t="s">
+      <c r="H5" s="24"/>
+      <c r="I5" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18" t="s">
+      <c r="J5" s="24"/>
+      <c r="K5" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="L5" s="18"/>
-      <c r="M5" s="18" t="s">
+      <c r="L5" s="24"/>
+      <c r="M5" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="N5" s="18"/>
+      <c r="N5" s="24"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C6" s="4">
@@ -1842,26 +1842,26 @@
       <c r="B8" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18" t="s">
+      <c r="D8" s="24"/>
+      <c r="E8" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18" t="s">
+      <c r="F8" s="24"/>
+      <c r="G8" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="H8" s="18"/>
-      <c r="I8" s="19" t="s">
+      <c r="H8" s="24"/>
+      <c r="I8" s="25" t="s">
         <v>108</v>
       </c>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20"/>
-      <c r="M8" s="20"/>
-      <c r="N8" s="21"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="26"/>
+      <c r="M8" s="26"/>
+      <c r="N8" s="27"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C9" s="4">
@@ -1897,22 +1897,22 @@
       <c r="B11" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="19" t="s">
+      <c r="D11" s="24"/>
+      <c r="E11" s="25" t="s">
         <v>109</v>
       </c>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="20"/>
-      <c r="M11" s="20"/>
-      <c r="N11" s="21"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="26"/>
+      <c r="M11" s="26"/>
+      <c r="N11" s="27"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C12" s="4">
@@ -1940,30 +1940,30 @@
       <c r="B16" t="s">
         <v>166</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18" t="s">
+      <c r="D16" s="24"/>
+      <c r="E16" s="24" t="s">
         <v>233</v>
       </c>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18" t="s">
+      <c r="F16" s="24"/>
+      <c r="G16" s="24" t="s">
         <v>234</v>
       </c>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18" t="s">
+      <c r="H16" s="24"/>
+      <c r="I16" s="24" t="s">
         <v>235</v>
       </c>
-      <c r="J16" s="18"/>
-      <c r="K16" s="18" t="s">
+      <c r="J16" s="24"/>
+      <c r="K16" s="24" t="s">
         <v>236</v>
       </c>
-      <c r="L16" s="18"/>
-      <c r="M16" s="18" t="s">
+      <c r="L16" s="24"/>
+      <c r="M16" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="N16" s="18"/>
+      <c r="N16" s="24"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C17" s="4">
@@ -2007,26 +2007,26 @@
       <c r="B19" t="s">
         <v>152</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18" t="s">
+      <c r="D19" s="24"/>
+      <c r="E19" s="24" t="s">
         <v>233</v>
       </c>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18" t="s">
+      <c r="F19" s="24"/>
+      <c r="G19" s="24" t="s">
         <v>234</v>
       </c>
-      <c r="H19" s="18"/>
-      <c r="I19" s="19" t="s">
+      <c r="H19" s="24"/>
+      <c r="I19" s="25" t="s">
         <v>108</v>
       </c>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="20"/>
-      <c r="M19" s="20"/>
-      <c r="N19" s="21"/>
+      <c r="J19" s="26"/>
+      <c r="K19" s="26"/>
+      <c r="L19" s="26"/>
+      <c r="M19" s="26"/>
+      <c r="N19" s="27"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C20" s="4">
@@ -2060,18 +2060,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:N11"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="I8:N8"/>
     <mergeCell ref="M16:N16"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="E19:F19"/>
@@ -2082,6 +2070,18 @@
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="I16:J16"/>
     <mergeCell ref="K16:L16"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:N11"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="I8:N8"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2091,8 +2091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:Z37"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2109,23 +2109,23 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="L2" s="22" t="s">
+      <c r="L2" s="28" t="s">
         <v>281</v>
       </c>
-      <c r="M2" s="22"/>
-      <c r="N2" s="22"/>
-      <c r="O2" s="22"/>
-      <c r="P2" s="22"/>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="22"/>
-      <c r="S2" s="22"/>
-      <c r="T2" s="22"/>
-      <c r="U2" s="22"/>
-      <c r="V2" s="22"/>
-      <c r="W2" s="22"/>
-      <c r="X2" s="22"/>
-      <c r="Y2" s="22"/>
-      <c r="Z2" s="22"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="28"/>
+      <c r="O2" s="28"/>
+      <c r="P2" s="28"/>
+      <c r="Q2" s="28"/>
+      <c r="R2" s="28"/>
+      <c r="S2" s="28"/>
+      <c r="T2" s="28"/>
+      <c r="U2" s="28"/>
+      <c r="V2" s="28"/>
+      <c r="W2" s="28"/>
+      <c r="X2" s="28"/>
+      <c r="Y2" s="28"/>
+      <c r="Z2" s="28"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -2187,7 +2187,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="29"/>
+      <c r="A4" s="23"/>
       <c r="B4" s="13">
         <v>1</v>
       </c>
@@ -2200,7 +2200,7 @@
       <c r="E4" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="F4" s="18" t="s">
         <v>7</v>
       </c>
       <c r="G4" s="14" t="s">
@@ -2245,7 +2245,7 @@
       <c r="T4" s="14"/>
     </row>
     <row r="5" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="29"/>
+      <c r="A5" s="23"/>
       <c r="B5" s="13">
         <f>B4+1</f>
         <v>2</v>
@@ -2330,7 +2330,7 @@
       <c r="T6" s="9"/>
     </row>
     <row r="7" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="29"/>
+      <c r="A7" s="23"/>
       <c r="B7" s="13">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -2344,7 +2344,7 @@
       <c r="E7" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="24" t="s">
+      <c r="F7" s="18" t="s">
         <v>25</v>
       </c>
       <c r="G7" s="14"/>
@@ -2371,7 +2371,7 @@
       <c r="T7" s="14"/>
     </row>
     <row r="8" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="29"/>
+      <c r="A8" s="23"/>
       <c r="B8" s="13">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -2414,7 +2414,7 @@
       <c r="T8" s="14"/>
     </row>
     <row r="9" spans="1:26" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="29"/>
+      <c r="A9" s="23"/>
       <c r="B9" s="13">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -2457,7 +2457,7 @@
       <c r="T9" s="14"/>
     </row>
     <row r="10" spans="1:26" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="29"/>
+      <c r="A10" s="23"/>
       <c r="B10" s="13">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -2500,7 +2500,7 @@
       <c r="T10" s="14"/>
     </row>
     <row r="11" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="29"/>
+      <c r="A11" s="23"/>
       <c r="B11" s="13">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -2537,7 +2537,7 @@
       <c r="T11" s="14"/>
     </row>
     <row r="12" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="29"/>
+      <c r="A12" s="23"/>
       <c r="B12" s="13">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -2574,7 +2574,7 @@
       <c r="T12" s="14"/>
     </row>
     <row r="13" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="29"/>
+      <c r="A13" s="23"/>
       <c r="B13" s="13">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -2588,7 +2588,7 @@
       <c r="E13" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="28" t="s">
+      <c r="F13" s="22" t="s">
         <v>273</v>
       </c>
       <c r="G13" s="14"/>
@@ -2611,7 +2611,7 @@
       <c r="T13" s="14"/>
     </row>
     <row r="14" spans="1:26" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="29"/>
+      <c r="A14" s="23"/>
       <c r="B14" s="13">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -2652,7 +2652,7 @@
       <c r="T14" s="14"/>
     </row>
     <row r="15" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="29"/>
+      <c r="A15" s="23"/>
       <c r="B15" s="13">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -2689,7 +2689,7 @@
       <c r="T15" s="14"/>
     </row>
     <row r="16" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="29"/>
+      <c r="A16" s="23"/>
       <c r="B16" s="13">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -2730,7 +2730,7 @@
       <c r="T16" s="14"/>
     </row>
     <row r="17" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="29"/>
+      <c r="A17" s="23"/>
       <c r="B17" s="13">
         <f>B16+1</f>
         <v>14</v>
@@ -2744,7 +2744,7 @@
       <c r="E17" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="26" t="s">
+      <c r="F17" s="20" t="s">
         <v>247</v>
       </c>
       <c r="G17" s="14"/>
@@ -2769,7 +2769,7 @@
       <c r="T17" s="14"/>
     </row>
     <row r="18" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="29"/>
+      <c r="A18" s="23"/>
       <c r="B18" s="13">
         <f>B16+1</f>
         <v>14</v>
@@ -2783,7 +2783,7 @@
       <c r="E18" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F18" s="24" t="s">
+      <c r="F18" s="18" t="s">
         <v>67</v>
       </c>
       <c r="G18" s="14"/>
@@ -2808,7 +2808,7 @@
       <c r="T18" s="14"/>
     </row>
     <row r="19" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="29"/>
+      <c r="A19" s="23"/>
       <c r="B19" s="13">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -2822,7 +2822,7 @@
       <c r="E19" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F19" s="24" t="s">
+      <c r="F19" s="18" t="s">
         <v>68</v>
       </c>
       <c r="G19" s="14"/>
@@ -2847,7 +2847,7 @@
       <c r="T19" s="14"/>
     </row>
     <row r="20" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="29"/>
+      <c r="A20" s="23"/>
       <c r="B20" s="13">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2886,7 +2886,7 @@
       <c r="T20" s="14"/>
     </row>
     <row r="21" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="29"/>
+      <c r="A21" s="23"/>
       <c r="B21" s="13">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2900,7 +2900,7 @@
       <c r="E21" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F21" s="24" t="s">
+      <c r="F21" s="18" t="s">
         <v>72</v>
       </c>
       <c r="G21" s="14"/>
@@ -2925,7 +2925,7 @@
       <c r="T21" s="14"/>
     </row>
     <row r="22" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="29"/>
+      <c r="A22" s="23"/>
       <c r="B22" s="13">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -2939,7 +2939,7 @@
       <c r="E22" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F22" s="24" t="s">
+      <c r="F22" s="18" t="s">
         <v>75</v>
       </c>
       <c r="G22" s="14" t="s">
@@ -2966,7 +2966,7 @@
       <c r="T22" s="14"/>
     </row>
     <row r="23" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="29"/>
+      <c r="A23" s="23"/>
       <c r="B23" s="13">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -2980,7 +2980,7 @@
       <c r="E23" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F23" s="25" t="s">
+      <c r="F23" s="19" t="s">
         <v>274</v>
       </c>
       <c r="G23" s="14"/>
@@ -3005,7 +3005,7 @@
       <c r="T23" s="14"/>
     </row>
     <row r="24" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="29"/>
+      <c r="A24" s="23"/>
       <c r="B24" s="13">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -3019,7 +3019,7 @@
       <c r="E24" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F24" s="25" t="s">
+      <c r="F24" s="19" t="s">
         <v>275</v>
       </c>
       <c r="G24" s="14"/>
@@ -3044,7 +3044,7 @@
       <c r="T24" s="14"/>
     </row>
     <row r="25" spans="1:20" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="29"/>
+      <c r="A25" s="23"/>
       <c r="B25" s="13">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -3083,7 +3083,7 @@
       <c r="T25" s="14"/>
     </row>
     <row r="26" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="29"/>
+      <c r="A26" s="23"/>
       <c r="B26" s="13">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -3122,7 +3122,7 @@
       <c r="T26" s="14"/>
     </row>
     <row r="27" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="29"/>
+      <c r="A27" s="23"/>
       <c r="B27" s="13">
         <f>B26+1</f>
         <v>23</v>
@@ -3136,7 +3136,7 @@
       <c r="E27" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F27" s="27" t="s">
+      <c r="F27" s="21" t="s">
         <v>244</v>
       </c>
       <c r="G27" s="14"/>
@@ -3159,7 +3159,7 @@
       <c r="T27" s="14"/>
     </row>
     <row r="28" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="29"/>
+      <c r="A28" s="23"/>
       <c r="B28" s="13">
         <f>B26+1</f>
         <v>23</v>
@@ -3173,7 +3173,7 @@
       <c r="E28" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F28" s="24" t="s">
+      <c r="F28" s="18" t="s">
         <v>241</v>
       </c>
       <c r="G28" s="14" t="s">
@@ -3198,7 +3198,7 @@
       <c r="T28" s="14"/>
     </row>
     <row r="29" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="29"/>
+      <c r="A29" s="23"/>
       <c r="B29" s="13">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -3212,7 +3212,7 @@
       <c r="E29" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F29" s="24" t="s">
+      <c r="F29" s="18" t="s">
         <v>241</v>
       </c>
       <c r="G29" s="14"/>
@@ -3503,7 +3503,7 @@
   <dimension ref="A3:N27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3540,7 +3540,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="29"/>
+      <c r="A4" s="23"/>
       <c r="B4" s="14" t="s">
         <v>150</v>
       </c>
@@ -3564,7 +3564,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="29"/>
+      <c r="A5" s="23"/>
       <c r="B5" s="14" t="s">
         <v>155</v>
       </c>
@@ -3588,7 +3588,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="29"/>
+      <c r="A6" s="23"/>
       <c r="B6" s="14" t="s">
         <v>159</v>
       </c>
@@ -3610,7 +3610,7 @@
       </c>
     </row>
     <row r="7" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="29"/>
+      <c r="A7" s="23"/>
       <c r="B7" s="14" t="s">
         <v>162</v>
       </c>
@@ -3634,7 +3634,7 @@
       </c>
     </row>
     <row r="8" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="29"/>
+      <c r="A8" s="23"/>
       <c r="B8" s="14" t="s">
         <v>164</v>
       </c>
@@ -3656,7 +3656,7 @@
       </c>
     </row>
     <row r="9" spans="1:14" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="29"/>
+      <c r="A9" s="23"/>
       <c r="B9" s="14" t="s">
         <v>169</v>
       </c>
@@ -3678,7 +3678,7 @@
       </c>
     </row>
     <row r="10" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="29"/>
+      <c r="A10" s="23"/>
       <c r="B10" s="14" t="s">
         <v>172</v>
       </c>
@@ -3703,7 +3703,7 @@
       </c>
     </row>
     <row r="11" spans="1:14" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="29"/>
+      <c r="A11" s="23"/>
       <c r="B11" s="14" t="s">
         <v>176</v>
       </c>
@@ -3763,13 +3763,13 @@
       <c r="G13" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="I13" s="23" t="s">
+      <c r="I13" s="29" t="s">
         <v>144</v>
       </c>
-      <c r="J13" s="23"/>
-      <c r="K13" s="23"/>
-      <c r="L13" s="23"/>
-      <c r="M13" s="23"/>
+      <c r="J13" s="29"/>
+      <c r="K13" s="29"/>
+      <c r="L13" s="29"/>
+      <c r="M13" s="29"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
@@ -3787,11 +3787,11 @@
       <c r="G14" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="I14" s="23"/>
-      <c r="J14" s="23"/>
-      <c r="K14" s="23"/>
-      <c r="L14" s="23"/>
-      <c r="M14" s="23"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="29"/>
+      <c r="K14" s="29"/>
+      <c r="L14" s="29"/>
+      <c r="M14" s="29"/>
     </row>
     <row r="15" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
@@ -3845,7 +3845,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="29"/>
+      <c r="A18" s="23"/>
       <c r="B18" s="14" t="s">
         <v>200</v>
       </c>
@@ -3869,7 +3869,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="29"/>
+      <c r="A19" s="23"/>
       <c r="B19" s="14" t="s">
         <v>204</v>
       </c>
@@ -3893,7 +3893,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="29"/>
+      <c r="A20" s="23"/>
       <c r="B20" s="14" t="s">
         <v>207</v>
       </c>
@@ -3903,7 +3903,7 @@
       <c r="D20" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E20" s="24" t="s">
+      <c r="E20" s="18" t="s">
         <v>209</v>
       </c>
       <c r="F20" s="14"/>
@@ -3915,7 +3915,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="29"/>
+      <c r="A21" s="23"/>
       <c r="B21" s="14" t="s">
         <v>210</v>
       </c>
@@ -3925,7 +3925,7 @@
       <c r="D21" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E21" s="24" t="s">
+      <c r="E21" s="18" t="s">
         <v>212</v>
       </c>
       <c r="F21" s="14"/>
@@ -3958,7 +3958,7 @@
       </c>
     </row>
     <row r="23" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="29"/>
+      <c r="A23" s="23"/>
       <c r="B23" s="14" t="s">
         <v>217</v>
       </c>
@@ -3980,7 +3980,7 @@
       </c>
     </row>
     <row r="24" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="29"/>
+      <c r="A24" s="23"/>
       <c r="B24" s="14" t="s">
         <v>220</v>
       </c>
@@ -4004,7 +4004,7 @@
       </c>
     </row>
     <row r="25" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="29"/>
+      <c r="A25" s="23"/>
       <c r="B25" s="14" t="s">
         <v>223</v>
       </c>
@@ -4014,7 +4014,7 @@
       <c r="D25" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E25" s="25" t="s">
+      <c r="E25" s="19" t="s">
         <v>225</v>
       </c>
       <c r="F25" s="14"/>
@@ -4026,7 +4026,7 @@
       </c>
     </row>
     <row r="26" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="29"/>
+      <c r="A26" s="23"/>
       <c r="B26" s="14" t="s">
         <v>226</v>
       </c>
@@ -4050,7 +4050,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="29"/>
+      <c r="A27" s="23"/>
       <c r="B27" s="14" t="s">
         <v>230</v>
       </c>

</xml_diff>